<commit_message>
balance times and resources
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitd\minute_empire\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B22A4-562E-4DC4-8F1F-3BF50B355280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4940251E-05DF-49DA-B52D-46130B10A60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
   </bookViews>
   <sheets>
     <sheet name="brainstorming" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
   <si>
     <t>Collections</t>
   </si>
@@ -301,6 +301,18 @@
   </si>
   <si>
     <t>GET https://fonts.googleapis.com/css2?family=Roboto:wght@100;300;400;500;700;900&amp;display=swap net::ERR_NAME_NOT_RESOLVED</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t>Slots do círculo externo são liberado quando centro da cidade atinge nível 5</t>
+  </si>
+  <si>
+    <t>Centro da cidade nível 5 precisa de pelo menos população 30</t>
+  </si>
+  <si>
+    <t>Custos das construções vai variar de acordo com o nível que eu quero que o pessoal construa ela</t>
   </si>
 </sst>
 </file>
@@ -1203,6 +1215,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1280,48 +1334,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1659,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160B8A5D-57A4-491A-8F64-525E78E348B7}">
   <dimension ref="A1:AU69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="AJ24" sqref="AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,34 +1936,34 @@
       </c>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="O28" s="66" t="s">
+      <c r="O28" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="P28" s="66"/>
-      <c r="Q28" s="66"/>
-      <c r="R28" s="66"/>
-      <c r="S28" s="66"/>
-      <c r="W28" s="66" t="s">
+      <c r="P28" s="80"/>
+      <c r="Q28" s="80"/>
+      <c r="R28" s="80"/>
+      <c r="S28" s="80"/>
+      <c r="W28" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="X28" s="66"/>
-      <c r="Y28" s="66"/>
-      <c r="Z28" s="66"/>
-      <c r="AA28" s="66"/>
-      <c r="AD28" s="66" t="s">
+      <c r="X28" s="80"/>
+      <c r="Y28" s="80"/>
+      <c r="Z28" s="80"/>
+      <c r="AA28" s="80"/>
+      <c r="AD28" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="AE28" s="66"/>
-      <c r="AF28" s="66"/>
-      <c r="AG28" s="66"/>
-      <c r="AH28" s="66"/>
-      <c r="AL28" s="66" t="s">
+      <c r="AE28" s="80"/>
+      <c r="AF28" s="80"/>
+      <c r="AG28" s="80"/>
+      <c r="AH28" s="80"/>
+      <c r="AL28" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="AM28" s="66"/>
-      <c r="AN28" s="66"/>
-      <c r="AO28" s="66"/>
-      <c r="AP28" s="66"/>
+      <c r="AM28" s="80"/>
+      <c r="AN28" s="80"/>
+      <c r="AO28" s="80"/>
+      <c r="AP28" s="80"/>
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="N29" s="19"/>
@@ -3732,97 +3744,109 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550AAB3F-C06C-4BC4-BC52-26C567DF5A60}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="72"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="86"/>
+      <c r="N1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="74"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="88"/>
+      <c r="N2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="74"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="88"/>
+      <c r="N3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="74"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="88"/>
+      <c r="N4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="74"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="88"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="69"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3841,8 +3865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA015092-742B-4B09-B582-52072BAD5DCA}">
   <dimension ref="G1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3851,10 +3875,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="66"/>
+      <c r="H1" s="80"/>
       <c r="K1" t="s">
         <v>53</v>
       </c>
@@ -3943,7 +3967,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L35" sqref="L35"/>
+      <selection pane="topRight" activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4042,93 +4066,93 @@
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="82" t="s">
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="92"/>
+      <c r="T3" s="92"/>
+      <c r="U3" s="92"/>
+      <c r="V3" s="92"/>
+      <c r="W3" s="92"/>
+      <c r="X3" s="92"/>
+      <c r="Y3" s="92"/>
+      <c r="Z3" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="82"/>
-      <c r="AB3" s="82"/>
-      <c r="AC3" s="82"/>
+      <c r="AA3" s="96"/>
+      <c r="AB3" s="96"/>
+      <c r="AC3" s="96"/>
       <c r="AD3" s="19"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78" t="s">
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
       <c r="J4" s="25"/>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
       <c r="O4" s="25"/>
-      <c r="P4" s="78" t="s">
+      <c r="P4" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
+      <c r="Q4" s="92"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="92"/>
       <c r="T4" s="25"/>
-      <c r="U4" s="78" t="s">
+      <c r="U4" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="82" t="s">
+      <c r="V4" s="92"/>
+      <c r="W4" s="92"/>
+      <c r="X4" s="92"/>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="82" t="s">
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="AC4" s="82"/>
-      <c r="AD4" s="78" t="s">
+      <c r="AC4" s="96"/>
+      <c r="AD4" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="78"/>
-      <c r="AG4" s="78"/>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78" t="s">
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
+      <c r="AH4" s="92"/>
+      <c r="AI4" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="78"/>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="78"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="92"/>
+      <c r="AL4" s="92"/>
+      <c r="AM4" s="92"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
@@ -4300,85 +4324,85 @@
       <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="89"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="89"/>
-      <c r="S8" s="89"/>
-      <c r="T8" s="89"/>
-      <c r="U8" s="89"/>
-      <c r="V8" s="89"/>
-      <c r="W8" s="89"/>
-      <c r="X8" s="89"/>
-      <c r="Y8" s="90"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="103"/>
+      <c r="X8" s="103"/>
+      <c r="Y8" s="104"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="83" t="s">
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="83" t="s">
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="83" t="s">
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="99"/>
+      <c r="P9" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="84"/>
-      <c r="R9" s="84"/>
-      <c r="S9" s="84"/>
-      <c r="T9" s="85"/>
-      <c r="U9" s="86" t="s">
+      <c r="Q9" s="98"/>
+      <c r="R9" s="98"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="99"/>
+      <c r="U9" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="87"/>
-      <c r="W9" s="87"/>
-      <c r="X9" s="87"/>
-      <c r="Y9" s="87"/>
-      <c r="Z9" s="79" t="s">
+      <c r="V9" s="101"/>
+      <c r="W9" s="101"/>
+      <c r="X9" s="101"/>
+      <c r="Y9" s="101"/>
+      <c r="Z9" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="80"/>
-      <c r="AB9" s="80"/>
-      <c r="AC9" s="81"/>
-      <c r="AD9" s="75" t="s">
+      <c r="AA9" s="94"/>
+      <c r="AB9" s="94"/>
+      <c r="AC9" s="95"/>
+      <c r="AD9" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="AE9" s="76"/>
-      <c r="AF9" s="76"/>
-      <c r="AG9" s="76"/>
-      <c r="AH9" s="77"/>
-      <c r="AI9" s="75" t="s">
+      <c r="AE9" s="90"/>
+      <c r="AF9" s="90"/>
+      <c r="AG9" s="90"/>
+      <c r="AH9" s="91"/>
+      <c r="AI9" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="AJ9" s="76"/>
-      <c r="AK9" s="76"/>
-      <c r="AL9" s="76"/>
-      <c r="AM9" s="77"/>
+      <c r="AJ9" s="90"/>
+      <c r="AK9" s="90"/>
+      <c r="AL9" s="90"/>
+      <c r="AM9" s="91"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
@@ -4503,122 +4527,122 @@
       <c r="A11" s="38">
         <v>0</v>
       </c>
-      <c r="B11" s="93">
+      <c r="B11" s="67">
         <v>100</v>
       </c>
-      <c r="C11" s="94">
+      <c r="C11" s="68">
         <v>100</v>
       </c>
-      <c r="D11" s="94">
+      <c r="D11" s="68">
         <v>100</v>
       </c>
-      <c r="E11" s="95">
+      <c r="E11" s="69">
         <v>100</v>
       </c>
-      <c r="F11" s="96">
-        <v>0</v>
-      </c>
-      <c r="G11" s="97">
+      <c r="F11" s="70">
+        <v>0</v>
+      </c>
+      <c r="G11" s="71">
         <v>25</v>
       </c>
-      <c r="H11" s="97">
+      <c r="H11" s="71">
         <v>25</v>
       </c>
-      <c r="I11" s="98">
+      <c r="I11" s="72">
         <v>15</v>
       </c>
-      <c r="J11" s="99">
+      <c r="J11" s="73">
         <v>2</v>
       </c>
-      <c r="K11" s="96">
-        <v>0</v>
-      </c>
-      <c r="L11" s="97">
+      <c r="K11" s="70">
+        <v>0</v>
+      </c>
+      <c r="L11" s="71">
         <v>30</v>
       </c>
-      <c r="M11" s="97">
+      <c r="M11" s="71">
         <v>40</v>
       </c>
-      <c r="N11" s="98">
+      <c r="N11" s="72">
         <v>20</v>
       </c>
-      <c r="O11" s="99">
+      <c r="O11" s="73">
         <v>2</v>
       </c>
-      <c r="P11" s="96">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="97">
+      <c r="P11" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="71">
         <v>40</v>
       </c>
-      <c r="R11" s="97">
+      <c r="R11" s="71">
         <v>30</v>
       </c>
-      <c r="S11" s="98">
+      <c r="S11" s="72">
         <v>25</v>
       </c>
-      <c r="T11" s="99">
+      <c r="T11" s="73">
         <v>2</v>
       </c>
-      <c r="U11" s="96">
-        <v>0</v>
-      </c>
-      <c r="V11" s="97">
+      <c r="U11" s="70">
+        <v>0</v>
+      </c>
+      <c r="V11" s="71">
         <v>50</v>
       </c>
-      <c r="W11" s="97">
+      <c r="W11" s="71">
         <v>60</v>
       </c>
-      <c r="X11" s="97">
+      <c r="X11" s="71">
         <v>30</v>
       </c>
-      <c r="Y11" s="99">
+      <c r="Y11" s="73">
         <v>2</v>
       </c>
-      <c r="Z11" s="100">
+      <c r="Z11" s="74">
         <f>$AA$5</f>
         <v>300</v>
       </c>
-      <c r="AA11" s="101">
+      <c r="AA11" s="75">
         <f>$AC$5</f>
         <v>300</v>
       </c>
-      <c r="AB11" s="101">
+      <c r="AB11" s="75">
         <f>$AC$5</f>
         <v>300</v>
       </c>
-      <c r="AC11" s="101">
+      <c r="AC11" s="75">
         <f>$AC$5</f>
         <v>300</v>
       </c>
-      <c r="AD11" s="102">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="102">
+      <c r="AD11" s="76">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="76">
         <v>60</v>
       </c>
-      <c r="AF11" s="102">
+      <c r="AF11" s="76">
         <v>75</v>
       </c>
-      <c r="AG11" s="103">
+      <c r="AG11" s="77">
         <v>40</v>
       </c>
-      <c r="AH11" s="104">
+      <c r="AH11" s="78">
         <v>3</v>
       </c>
-      <c r="AI11" s="105">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="102">
+      <c r="AI11" s="79">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="76">
         <v>70</v>
       </c>
-      <c r="AK11" s="102">
+      <c r="AK11" s="76">
         <v>90</v>
       </c>
-      <c r="AL11" s="103">
+      <c r="AL11" s="77">
         <v>50</v>
       </c>
-      <c r="AM11" s="104">
+      <c r="AM11" s="78">
         <v>4</v>
       </c>
     </row>
@@ -4627,19 +4651,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="39">
-        <f>B11+B$5*$C$2^($A12)</f>
+        <f t="shared" ref="B12:B26" si="0">B11+B$5*$C$2^($A12)</f>
         <v>220</v>
       </c>
       <c r="C12" s="26">
-        <f>C11+C$5*$C$2^($A12)</f>
+        <f t="shared" ref="C12:C26" si="1">C11+C$5*$C$2^($A12)</f>
         <v>244</v>
       </c>
       <c r="D12" s="26">
-        <f>D11+D$5*$C$2^($A12)</f>
+        <f t="shared" ref="D12:D26" si="2">D11+D$5*$C$2^($A12)</f>
         <v>220</v>
       </c>
       <c r="E12" s="40">
-        <f>E11+E$5*$C$2^($A12)</f>
+        <f t="shared" ref="E12:E26" si="3">E11+E$5*$C$2^($A12)</f>
         <v>196</v>
       </c>
       <c r="F12" s="31">
@@ -4663,19 +4687,19 @@
         <v>1.42</v>
       </c>
       <c r="K12" s="31">
-        <f t="shared" ref="K12:X12" si="0">K$5*$G$2^($A12)</f>
+        <f t="shared" ref="K12:X12" si="4">K$5*$G$2^($A12)</f>
         <v>0</v>
       </c>
       <c r="L12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="M12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="N12" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="O12" s="45">
@@ -4683,19 +4707,19 @@
         <v>1.42</v>
       </c>
       <c r="P12" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="R12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="S12" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="T12" s="45">
@@ -4703,19 +4727,19 @@
         <v>1.42</v>
       </c>
       <c r="U12" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="W12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="X12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="Y12" s="45">
@@ -4731,11 +4755,11 @@
         <v>491.99999999999994</v>
       </c>
       <c r="AB12" s="19">
-        <f t="shared" ref="AB12:AC26" si="1">$AC$5*($AC$6^($A12))</f>
+        <f t="shared" ref="AB12:AC26" si="5">$AC$5*($AC$6^($A12))</f>
         <v>491.99999999999994</v>
       </c>
       <c r="AC12" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>491.99999999999994</v>
       </c>
       <c r="AD12" s="51">
@@ -4747,11 +4771,11 @@
         <v>270</v>
       </c>
       <c r="AF12" s="51">
-        <f t="shared" ref="AE12:AG26" si="2">AF$5*$AE$2^($A12)</f>
+        <f t="shared" ref="AE12:AG26" si="6">AF$5*$AE$2^($A12)</f>
         <v>210</v>
       </c>
       <c r="AG12" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="AH12" s="58">
@@ -4763,11 +4787,11 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="51">
-        <f t="shared" ref="AJ12:AL26" si="3">AJ$5*$AJ$2^($A12)</f>
+        <f t="shared" ref="AJ12:AL26" si="7">AJ$5*$AJ$2^($A12)</f>
         <v>300</v>
       </c>
       <c r="AK12" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="AL12" s="57">
@@ -4784,155 +4808,155 @@
         <v>2</v>
       </c>
       <c r="B13" s="39">
-        <f>B12+B$5*$C$2^($A13)</f>
+        <f t="shared" si="0"/>
         <v>364</v>
       </c>
       <c r="C13" s="26">
-        <f>C12+C$5*$C$2^($A13)</f>
+        <f t="shared" si="1"/>
         <v>416.79999999999995</v>
       </c>
       <c r="D13" s="26">
-        <f>D12+D$5*$C$2^($A13)</f>
+        <f t="shared" si="2"/>
         <v>364</v>
       </c>
       <c r="E13" s="40">
-        <f>E12+E$5*$C$2^($A13)</f>
+        <f t="shared" si="3"/>
         <v>311.2</v>
       </c>
       <c r="F13" s="31">
-        <f t="shared" ref="F13:X26" si="4">F$5*$G$2^($A13)</f>
+        <f t="shared" ref="F13:X26" si="8">F$5*$G$2^($A13)</f>
         <v>0</v>
       </c>
       <c r="G13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="H13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="I13" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="J13" s="45">
-        <f t="shared" ref="J13:J26" si="5">J$5*$J$2^($A13)</f>
+        <f t="shared" ref="J13:J26" si="9">J$5*$J$2^($A13)</f>
         <v>2.0164</v>
       </c>
       <c r="K13" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>225</v>
       </c>
       <c r="M13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="N13" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="O13" s="45">
-        <f t="shared" ref="O13:O26" si="6">O$5*$J$2^($A13)</f>
+        <f t="shared" ref="O13:O26" si="10">O$5*$J$2^($A13)</f>
         <v>2.0164</v>
       </c>
       <c r="P13" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="R13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>225</v>
       </c>
       <c r="S13" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="T13" s="45">
-        <f t="shared" ref="T13:T26" si="7">T$5*$J$2^($A13)</f>
+        <f t="shared" ref="T13:T26" si="11">T$5*$J$2^($A13)</f>
         <v>2.0164</v>
       </c>
       <c r="U13" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="W13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="X13" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>225</v>
       </c>
       <c r="Y13" s="45">
-        <f t="shared" ref="Y13:Y26" si="8">Y$5*$J$2^($A13)</f>
+        <f t="shared" ref="Y13:Y26" si="12">Y$5*$J$2^($A13)</f>
         <v>2.0164</v>
       </c>
       <c r="Z13" s="52">
-        <f t="shared" ref="Z13:Z26" si="9">$AA$5*($AA$6^($A13))</f>
+        <f t="shared" ref="Z13:Z26" si="13">$AA$5*($AA$6^($A13))</f>
         <v>806.87999999999988</v>
       </c>
       <c r="AA13" s="19">
-        <f t="shared" ref="AA13:AA26" si="10">$AC$5*($AC$6^($A13))</f>
+        <f t="shared" ref="AA13:AA26" si="14">$AC$5*($AC$6^($A13))</f>
         <v>806.87999999999988</v>
       </c>
       <c r="AB13" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>806.87999999999988</v>
       </c>
       <c r="AC13" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>806.87999999999988</v>
       </c>
       <c r="AD13" s="51">
-        <f t="shared" ref="AD13:AD26" si="11">AD$5*$AE$2^($A13)</f>
+        <f t="shared" ref="AD13:AD26" si="15">AD$5*$AE$2^($A13)</f>
         <v>0</v>
       </c>
       <c r="AE13" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>405</v>
       </c>
       <c r="AF13" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>315</v>
       </c>
       <c r="AG13" s="57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>225</v>
       </c>
       <c r="AH13" s="58">
-        <f t="shared" ref="AH13:AH26" si="12">AH$5*$AG$2^($A13)</f>
+        <f t="shared" ref="AH13:AH26" si="16">AH$5*$AG$2^($A13)</f>
         <v>6.1504000000000003</v>
       </c>
       <c r="AI13" s="65">
-        <f t="shared" ref="AI13:AI26" si="13">$AI12*$AJ$2^($A13)</f>
+        <f t="shared" ref="AI13:AI26" si="17">$AI12*$AJ$2^($A13)</f>
         <v>0</v>
       </c>
       <c r="AJ13" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>450</v>
       </c>
       <c r="AK13" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>360</v>
       </c>
       <c r="AL13" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>270</v>
       </c>
       <c r="AM13" s="58">
-        <f t="shared" ref="AM13:AM26" si="14">AM$5*$AL$2^($A13)</f>
+        <f t="shared" ref="AM13:AM26" si="18">AM$5*$AL$2^($A13)</f>
         <v>8.64</v>
       </c>
     </row>
@@ -4941,155 +4965,155 @@
         <v>3</v>
       </c>
       <c r="B14" s="39">
-        <f>B13+B$5*$C$2^($A14)</f>
+        <f t="shared" si="0"/>
         <v>536.79999999999995</v>
       </c>
       <c r="C14" s="26">
-        <f>C13+C$5*$C$2^($A14)</f>
+        <f t="shared" si="1"/>
         <v>624.16</v>
       </c>
       <c r="D14" s="26">
-        <f>D13+D$5*$C$2^($A14)</f>
+        <f t="shared" si="2"/>
         <v>536.79999999999995</v>
       </c>
       <c r="E14" s="40">
-        <f>E13+E$5*$C$2^($A14)</f>
+        <f t="shared" si="3"/>
         <v>449.44</v>
       </c>
       <c r="F14" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G14" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>270</v>
       </c>
       <c r="H14" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>202.5</v>
       </c>
       <c r="I14" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>202.5</v>
       </c>
       <c r="J14" s="45">
+        <f t="shared" si="9"/>
+        <v>2.8632879999999998</v>
+      </c>
+      <c r="K14" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="32">
+        <f t="shared" si="8"/>
+        <v>337.5</v>
+      </c>
+      <c r="M14" s="32">
+        <f t="shared" si="8"/>
+        <v>270</v>
+      </c>
+      <c r="N14" s="33">
+        <f t="shared" si="8"/>
+        <v>202.5</v>
+      </c>
+      <c r="O14" s="45">
+        <f t="shared" si="10"/>
+        <v>2.8632879999999998</v>
+      </c>
+      <c r="P14" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="32">
+        <f t="shared" si="8"/>
+        <v>270</v>
+      </c>
+      <c r="R14" s="32">
+        <f t="shared" si="8"/>
+        <v>337.5</v>
+      </c>
+      <c r="S14" s="33">
+        <f t="shared" si="8"/>
+        <v>202.5</v>
+      </c>
+      <c r="T14" s="45">
+        <f t="shared" si="11"/>
+        <v>2.8632879999999998</v>
+      </c>
+      <c r="U14" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="32">
+        <f t="shared" si="8"/>
+        <v>202.5</v>
+      </c>
+      <c r="W14" s="32">
+        <f t="shared" si="8"/>
+        <v>270</v>
+      </c>
+      <c r="X14" s="32">
+        <f t="shared" si="8"/>
+        <v>337.5</v>
+      </c>
+      <c r="Y14" s="45">
+        <f t="shared" si="12"/>
+        <v>2.8632879999999998</v>
+      </c>
+      <c r="Z14" s="52">
+        <f t="shared" si="13"/>
+        <v>1323.2831999999996</v>
+      </c>
+      <c r="AA14" s="19">
+        <f t="shared" si="14"/>
+        <v>1323.2831999999996</v>
+      </c>
+      <c r="AB14" s="19">
         <f t="shared" si="5"/>
-        <v>2.8632879999999998</v>
-      </c>
-      <c r="K14" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="32">
-        <f t="shared" si="4"/>
+        <v>1323.2831999999996</v>
+      </c>
+      <c r="AC14" s="19">
+        <f t="shared" si="5"/>
+        <v>1323.2831999999996</v>
+      </c>
+      <c r="AD14" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="51">
+        <f t="shared" si="6"/>
+        <v>607.5</v>
+      </c>
+      <c r="AF14" s="51">
+        <f t="shared" si="6"/>
+        <v>472.5</v>
+      </c>
+      <c r="AG14" s="57">
+        <f t="shared" si="6"/>
         <v>337.5</v>
       </c>
-      <c r="M14" s="32">
-        <f t="shared" si="4"/>
-        <v>270</v>
-      </c>
-      <c r="N14" s="33">
-        <f t="shared" si="4"/>
-        <v>202.5</v>
-      </c>
-      <c r="O14" s="45">
-        <f t="shared" si="6"/>
-        <v>2.8632879999999998</v>
-      </c>
-      <c r="P14" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="32">
-        <f t="shared" si="4"/>
-        <v>270</v>
-      </c>
-      <c r="R14" s="32">
-        <f t="shared" si="4"/>
-        <v>337.5</v>
-      </c>
-      <c r="S14" s="33">
-        <f t="shared" si="4"/>
-        <v>202.5</v>
-      </c>
-      <c r="T14" s="45">
+      <c r="AH14" s="58">
+        <f t="shared" si="16"/>
+        <v>7.6264960000000004</v>
+      </c>
+      <c r="AI14" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="51">
         <f t="shared" si="7"/>
-        <v>2.8632879999999998</v>
-      </c>
-      <c r="U14" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="32">
-        <f t="shared" si="4"/>
-        <v>202.5</v>
-      </c>
-      <c r="W14" s="32">
-        <f t="shared" si="4"/>
-        <v>270</v>
-      </c>
-      <c r="X14" s="32">
-        <f t="shared" si="4"/>
-        <v>337.5</v>
-      </c>
-      <c r="Y14" s="45">
-        <f t="shared" si="8"/>
-        <v>2.8632879999999998</v>
-      </c>
-      <c r="Z14" s="52">
-        <f t="shared" si="9"/>
-        <v>1323.2831999999996</v>
-      </c>
-      <c r="AA14" s="19">
-        <f t="shared" si="10"/>
-        <v>1323.2831999999996</v>
-      </c>
-      <c r="AB14" s="19">
-        <f t="shared" si="1"/>
-        <v>1323.2831999999996</v>
-      </c>
-      <c r="AC14" s="19">
-        <f t="shared" si="1"/>
-        <v>1323.2831999999996</v>
-      </c>
-      <c r="AD14" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE14" s="51">
-        <f t="shared" si="2"/>
-        <v>607.5</v>
-      </c>
-      <c r="AF14" s="51">
-        <f t="shared" si="2"/>
-        <v>472.5</v>
-      </c>
-      <c r="AG14" s="57">
-        <f t="shared" si="2"/>
-        <v>337.5</v>
-      </c>
-      <c r="AH14" s="58">
-        <f t="shared" si="12"/>
-        <v>7.6264960000000004</v>
-      </c>
-      <c r="AI14" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="51">
-        <f t="shared" si="3"/>
         <v>675</v>
       </c>
       <c r="AK14" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>540</v>
       </c>
       <c r="AL14" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>405</v>
       </c>
       <c r="AM14" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>10.368</v>
       </c>
     </row>
@@ -5098,155 +5122,155 @@
         <v>4</v>
       </c>
       <c r="B15" s="39">
-        <f>B14+B$5*$C$2^($A15)</f>
+        <f t="shared" si="0"/>
         <v>744.16</v>
       </c>
       <c r="C15" s="26">
-        <f>C14+C$5*$C$2^($A15)</f>
+        <f t="shared" si="1"/>
         <v>872.99199999999996</v>
       </c>
       <c r="D15" s="26">
-        <f>D14+D$5*$C$2^($A15)</f>
+        <f t="shared" si="2"/>
         <v>744.16</v>
       </c>
       <c r="E15" s="40">
-        <f>E14+E$5*$C$2^($A15)</f>
+        <f t="shared" si="3"/>
         <v>615.32799999999997</v>
       </c>
       <c r="F15" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G15" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>405</v>
       </c>
       <c r="H15" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>303.75</v>
       </c>
       <c r="I15" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>303.75</v>
       </c>
       <c r="J15" s="45">
+        <f t="shared" si="9"/>
+        <v>4.0658689599999995</v>
+      </c>
+      <c r="K15" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="32">
+        <f t="shared" si="8"/>
+        <v>506.25</v>
+      </c>
+      <c r="M15" s="32">
+        <f t="shared" si="8"/>
+        <v>405</v>
+      </c>
+      <c r="N15" s="33">
+        <f t="shared" si="8"/>
+        <v>303.75</v>
+      </c>
+      <c r="O15" s="45">
+        <f t="shared" si="10"/>
+        <v>4.0658689599999995</v>
+      </c>
+      <c r="P15" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="32">
+        <f t="shared" si="8"/>
+        <v>405</v>
+      </c>
+      <c r="R15" s="32">
+        <f t="shared" si="8"/>
+        <v>506.25</v>
+      </c>
+      <c r="S15" s="33">
+        <f t="shared" si="8"/>
+        <v>303.75</v>
+      </c>
+      <c r="T15" s="45">
+        <f t="shared" si="11"/>
+        <v>4.0658689599999995</v>
+      </c>
+      <c r="U15" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="32">
+        <f t="shared" si="8"/>
+        <v>303.75</v>
+      </c>
+      <c r="W15" s="32">
+        <f t="shared" si="8"/>
+        <v>405</v>
+      </c>
+      <c r="X15" s="32">
+        <f t="shared" si="8"/>
+        <v>506.25</v>
+      </c>
+      <c r="Y15" s="45">
+        <f t="shared" si="12"/>
+        <v>4.0658689599999995</v>
+      </c>
+      <c r="Z15" s="52">
+        <f t="shared" si="13"/>
+        <v>2170.1844479999995</v>
+      </c>
+      <c r="AA15" s="19">
+        <f t="shared" si="14"/>
+        <v>2170.1844479999995</v>
+      </c>
+      <c r="AB15" s="19">
         <f t="shared" si="5"/>
-        <v>4.0658689599999995</v>
-      </c>
-      <c r="K15" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="32">
-        <f t="shared" si="4"/>
+        <v>2170.1844479999995</v>
+      </c>
+      <c r="AC15" s="19">
+        <f t="shared" si="5"/>
+        <v>2170.1844479999995</v>
+      </c>
+      <c r="AD15" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="51">
+        <f t="shared" si="6"/>
+        <v>911.25</v>
+      </c>
+      <c r="AF15" s="51">
+        <f t="shared" si="6"/>
+        <v>708.75</v>
+      </c>
+      <c r="AG15" s="57">
+        <f t="shared" si="6"/>
         <v>506.25</v>
       </c>
-      <c r="M15" s="32">
-        <f t="shared" si="4"/>
-        <v>405</v>
-      </c>
-      <c r="N15" s="33">
-        <f t="shared" si="4"/>
-        <v>303.75</v>
-      </c>
-      <c r="O15" s="45">
-        <f t="shared" si="6"/>
-        <v>4.0658689599999995</v>
-      </c>
-      <c r="P15" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="32">
-        <f t="shared" si="4"/>
-        <v>405</v>
-      </c>
-      <c r="R15" s="32">
-        <f t="shared" si="4"/>
-        <v>506.25</v>
-      </c>
-      <c r="S15" s="33">
-        <f t="shared" si="4"/>
-        <v>303.75</v>
-      </c>
-      <c r="T15" s="45">
+      <c r="AH15" s="58">
+        <f t="shared" si="16"/>
+        <v>9.4568550400000007</v>
+      </c>
+      <c r="AI15" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="51">
         <f t="shared" si="7"/>
-        <v>4.0658689599999995</v>
-      </c>
-      <c r="U15" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V15" s="32">
-        <f t="shared" si="4"/>
-        <v>303.75</v>
-      </c>
-      <c r="W15" s="32">
-        <f t="shared" si="4"/>
-        <v>405</v>
-      </c>
-      <c r="X15" s="32">
-        <f t="shared" si="4"/>
-        <v>506.25</v>
-      </c>
-      <c r="Y15" s="45">
-        <f t="shared" si="8"/>
-        <v>4.0658689599999995</v>
-      </c>
-      <c r="Z15" s="52">
-        <f t="shared" si="9"/>
-        <v>2170.1844479999995</v>
-      </c>
-      <c r="AA15" s="19">
-        <f t="shared" si="10"/>
-        <v>2170.1844479999995</v>
-      </c>
-      <c r="AB15" s="19">
-        <f t="shared" si="1"/>
-        <v>2170.1844479999995</v>
-      </c>
-      <c r="AC15" s="19">
-        <f t="shared" si="1"/>
-        <v>2170.1844479999995</v>
-      </c>
-      <c r="AD15" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE15" s="51">
-        <f t="shared" si="2"/>
-        <v>911.25</v>
-      </c>
-      <c r="AF15" s="51">
-        <f t="shared" si="2"/>
-        <v>708.75</v>
-      </c>
-      <c r="AG15" s="57">
-        <f t="shared" si="2"/>
-        <v>506.25</v>
-      </c>
-      <c r="AH15" s="58">
-        <f t="shared" si="12"/>
-        <v>9.4568550400000007</v>
-      </c>
-      <c r="AI15" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="51">
-        <f t="shared" si="3"/>
         <v>1012.5</v>
       </c>
       <c r="AK15" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>810</v>
       </c>
       <c r="AL15" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>607.5</v>
       </c>
       <c r="AM15" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>12.441599999999999</v>
       </c>
     </row>
@@ -5255,155 +5279,155 @@
         <v>5</v>
       </c>
       <c r="B16" s="39">
-        <f>B15+B$5*$C$2^($A16)</f>
+        <f t="shared" si="0"/>
         <v>992.99199999999996</v>
       </c>
       <c r="C16" s="26">
-        <f>C15+C$5*$C$2^($A16)</f>
+        <f t="shared" si="1"/>
         <v>1171.5904</v>
       </c>
       <c r="D16" s="26">
-        <f>D15+D$5*$C$2^($A16)</f>
+        <f t="shared" si="2"/>
         <v>992.99199999999996</v>
       </c>
       <c r="E16" s="40">
-        <f>E15+E$5*$C$2^($A16)</f>
+        <f t="shared" si="3"/>
         <v>814.39359999999999</v>
       </c>
       <c r="F16" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>607.5</v>
       </c>
       <c r="H16" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>455.625</v>
       </c>
       <c r="I16" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>455.625</v>
       </c>
       <c r="J16" s="45">
+        <f t="shared" si="9"/>
+        <v>5.7735339231999987</v>
+      </c>
+      <c r="K16" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="32">
+        <f t="shared" si="8"/>
+        <v>759.375</v>
+      </c>
+      <c r="M16" s="32">
+        <f t="shared" si="8"/>
+        <v>607.5</v>
+      </c>
+      <c r="N16" s="33">
+        <f t="shared" si="8"/>
+        <v>455.625</v>
+      </c>
+      <c r="O16" s="45">
+        <f t="shared" si="10"/>
+        <v>5.7735339231999987</v>
+      </c>
+      <c r="P16" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="32">
+        <f t="shared" si="8"/>
+        <v>607.5</v>
+      </c>
+      <c r="R16" s="32">
+        <f t="shared" si="8"/>
+        <v>759.375</v>
+      </c>
+      <c r="S16" s="33">
+        <f t="shared" si="8"/>
+        <v>455.625</v>
+      </c>
+      <c r="T16" s="45">
+        <f t="shared" si="11"/>
+        <v>5.7735339231999987</v>
+      </c>
+      <c r="U16" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="32">
+        <f t="shared" si="8"/>
+        <v>455.625</v>
+      </c>
+      <c r="W16" s="32">
+        <f t="shared" si="8"/>
+        <v>607.5</v>
+      </c>
+      <c r="X16" s="32">
+        <f t="shared" si="8"/>
+        <v>759.375</v>
+      </c>
+      <c r="Y16" s="45">
+        <f t="shared" si="12"/>
+        <v>5.7735339231999987</v>
+      </c>
+      <c r="Z16" s="52">
+        <f t="shared" si="13"/>
+        <v>3559.1024947199985</v>
+      </c>
+      <c r="AA16" s="19">
+        <f t="shared" si="14"/>
+        <v>3559.1024947199985</v>
+      </c>
+      <c r="AB16" s="19">
         <f t="shared" si="5"/>
-        <v>5.7735339231999987</v>
-      </c>
-      <c r="K16" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="32">
-        <f t="shared" si="4"/>
+        <v>3559.1024947199985</v>
+      </c>
+      <c r="AC16" s="19">
+        <f t="shared" si="5"/>
+        <v>3559.1024947199985</v>
+      </c>
+      <c r="AD16" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="51">
+        <f t="shared" si="6"/>
+        <v>1366.875</v>
+      </c>
+      <c r="AF16" s="51">
+        <f t="shared" si="6"/>
+        <v>1063.125</v>
+      </c>
+      <c r="AG16" s="57">
+        <f t="shared" si="6"/>
         <v>759.375</v>
       </c>
-      <c r="M16" s="32">
-        <f t="shared" si="4"/>
-        <v>607.5</v>
-      </c>
-      <c r="N16" s="33">
-        <f t="shared" si="4"/>
-        <v>455.625</v>
-      </c>
-      <c r="O16" s="45">
-        <f t="shared" si="6"/>
-        <v>5.7735339231999987</v>
-      </c>
-      <c r="P16" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="32">
-        <f t="shared" si="4"/>
-        <v>607.5</v>
-      </c>
-      <c r="R16" s="32">
-        <f t="shared" si="4"/>
-        <v>759.375</v>
-      </c>
-      <c r="S16" s="33">
-        <f t="shared" si="4"/>
-        <v>455.625</v>
-      </c>
-      <c r="T16" s="45">
+      <c r="AH16" s="58">
+        <f t="shared" si="16"/>
+        <v>11.726500249600001</v>
+      </c>
+      <c r="AI16" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="51">
         <f t="shared" si="7"/>
-        <v>5.7735339231999987</v>
-      </c>
-      <c r="U16" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V16" s="32">
-        <f t="shared" si="4"/>
-        <v>455.625</v>
-      </c>
-      <c r="W16" s="32">
-        <f t="shared" si="4"/>
-        <v>607.5</v>
-      </c>
-      <c r="X16" s="32">
-        <f t="shared" si="4"/>
-        <v>759.375</v>
-      </c>
-      <c r="Y16" s="45">
-        <f t="shared" si="8"/>
-        <v>5.7735339231999987</v>
-      </c>
-      <c r="Z16" s="52">
-        <f t="shared" si="9"/>
-        <v>3559.1024947199985</v>
-      </c>
-      <c r="AA16" s="19">
-        <f t="shared" si="10"/>
-        <v>3559.1024947199985</v>
-      </c>
-      <c r="AB16" s="19">
-        <f t="shared" si="1"/>
-        <v>3559.1024947199985</v>
-      </c>
-      <c r="AC16" s="19">
-        <f t="shared" si="1"/>
-        <v>3559.1024947199985</v>
-      </c>
-      <c r="AD16" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE16" s="51">
-        <f t="shared" si="2"/>
-        <v>1366.875</v>
-      </c>
-      <c r="AF16" s="51">
-        <f t="shared" si="2"/>
-        <v>1063.125</v>
-      </c>
-      <c r="AG16" s="57">
-        <f t="shared" si="2"/>
-        <v>759.375</v>
-      </c>
-      <c r="AH16" s="58">
-        <f t="shared" si="12"/>
-        <v>11.726500249600001</v>
-      </c>
-      <c r="AI16" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="51">
-        <f t="shared" si="3"/>
         <v>1518.75</v>
       </c>
       <c r="AK16" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1215</v>
       </c>
       <c r="AL16" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>911.25</v>
       </c>
       <c r="AM16" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>14.929919999999999</v>
       </c>
     </row>
@@ -5412,155 +5436,155 @@
         <v>6</v>
       </c>
       <c r="B17" s="39">
-        <f>B16+B$5*$C$2^($A17)</f>
+        <f t="shared" si="0"/>
         <v>1291.5904</v>
       </c>
       <c r="C17" s="26">
-        <f>C16+C$5*$C$2^($A17)</f>
+        <f t="shared" si="1"/>
         <v>1529.9084800000001</v>
       </c>
       <c r="D17" s="26">
-        <f>D16+D$5*$C$2^($A17)</f>
+        <f t="shared" si="2"/>
         <v>1291.5904</v>
       </c>
       <c r="E17" s="40">
-        <f>E16+E$5*$C$2^($A17)</f>
+        <f t="shared" si="3"/>
         <v>1053.27232</v>
       </c>
       <c r="F17" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G17" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>911.25</v>
       </c>
       <c r="H17" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>683.4375</v>
       </c>
       <c r="I17" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>683.4375</v>
       </c>
       <c r="J17" s="45">
+        <f t="shared" si="9"/>
+        <v>8.1984181709439987</v>
+      </c>
+      <c r="K17" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="32">
+        <f t="shared" si="8"/>
+        <v>1139.0625</v>
+      </c>
+      <c r="M17" s="32">
+        <f t="shared" si="8"/>
+        <v>911.25</v>
+      </c>
+      <c r="N17" s="33">
+        <f t="shared" si="8"/>
+        <v>683.4375</v>
+      </c>
+      <c r="O17" s="45">
+        <f t="shared" si="10"/>
+        <v>8.1984181709439987</v>
+      </c>
+      <c r="P17" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="32">
+        <f t="shared" si="8"/>
+        <v>911.25</v>
+      </c>
+      <c r="R17" s="32">
+        <f t="shared" si="8"/>
+        <v>1139.0625</v>
+      </c>
+      <c r="S17" s="33">
+        <f t="shared" si="8"/>
+        <v>683.4375</v>
+      </c>
+      <c r="T17" s="45">
+        <f t="shared" si="11"/>
+        <v>8.1984181709439987</v>
+      </c>
+      <c r="U17" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="32">
+        <f t="shared" si="8"/>
+        <v>683.4375</v>
+      </c>
+      <c r="W17" s="32">
+        <f t="shared" si="8"/>
+        <v>911.25</v>
+      </c>
+      <c r="X17" s="32">
+        <f t="shared" si="8"/>
+        <v>1139.0625</v>
+      </c>
+      <c r="Y17" s="45">
+        <f t="shared" si="12"/>
+        <v>8.1984181709439987</v>
+      </c>
+      <c r="Z17" s="52">
+        <f t="shared" si="13"/>
+        <v>5836.9280913407965</v>
+      </c>
+      <c r="AA17" s="19">
+        <f t="shared" si="14"/>
+        <v>5836.9280913407965</v>
+      </c>
+      <c r="AB17" s="19">
         <f t="shared" si="5"/>
-        <v>8.1984181709439987</v>
-      </c>
-      <c r="K17" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="32">
-        <f t="shared" si="4"/>
+        <v>5836.9280913407965</v>
+      </c>
+      <c r="AC17" s="19">
+        <f t="shared" si="5"/>
+        <v>5836.9280913407965</v>
+      </c>
+      <c r="AD17" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="51">
+        <f t="shared" si="6"/>
+        <v>2050.3125</v>
+      </c>
+      <c r="AF17" s="51">
+        <f t="shared" si="6"/>
+        <v>1594.6875</v>
+      </c>
+      <c r="AG17" s="57">
+        <f t="shared" si="6"/>
         <v>1139.0625</v>
       </c>
-      <c r="M17" s="32">
-        <f t="shared" si="4"/>
-        <v>911.25</v>
-      </c>
-      <c r="N17" s="33">
-        <f t="shared" si="4"/>
-        <v>683.4375</v>
-      </c>
-      <c r="O17" s="45">
-        <f t="shared" si="6"/>
-        <v>8.1984181709439987</v>
-      </c>
-      <c r="P17" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="32">
-        <f t="shared" si="4"/>
-        <v>911.25</v>
-      </c>
-      <c r="R17" s="32">
-        <f t="shared" si="4"/>
-        <v>1139.0625</v>
-      </c>
-      <c r="S17" s="33">
-        <f t="shared" si="4"/>
-        <v>683.4375</v>
-      </c>
-      <c r="T17" s="45">
+      <c r="AH17" s="58">
+        <f t="shared" si="16"/>
+        <v>14.540860309504001</v>
+      </c>
+      <c r="AI17" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="51">
         <f t="shared" si="7"/>
-        <v>8.1984181709439987</v>
-      </c>
-      <c r="U17" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V17" s="32">
-        <f t="shared" si="4"/>
-        <v>683.4375</v>
-      </c>
-      <c r="W17" s="32">
-        <f t="shared" si="4"/>
-        <v>911.25</v>
-      </c>
-      <c r="X17" s="32">
-        <f t="shared" si="4"/>
-        <v>1139.0625</v>
-      </c>
-      <c r="Y17" s="45">
-        <f t="shared" si="8"/>
-        <v>8.1984181709439987</v>
-      </c>
-      <c r="Z17" s="52">
-        <f t="shared" si="9"/>
-        <v>5836.9280913407965</v>
-      </c>
-      <c r="AA17" s="19">
-        <f t="shared" si="10"/>
-        <v>5836.9280913407965</v>
-      </c>
-      <c r="AB17" s="19">
-        <f t="shared" si="1"/>
-        <v>5836.9280913407965</v>
-      </c>
-      <c r="AC17" s="19">
-        <f t="shared" si="1"/>
-        <v>5836.9280913407965</v>
-      </c>
-      <c r="AD17" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE17" s="51">
-        <f t="shared" si="2"/>
-        <v>2050.3125</v>
-      </c>
-      <c r="AF17" s="51">
-        <f t="shared" si="2"/>
-        <v>1594.6875</v>
-      </c>
-      <c r="AG17" s="57">
-        <f t="shared" si="2"/>
-        <v>1139.0625</v>
-      </c>
-      <c r="AH17" s="58">
-        <f t="shared" si="12"/>
-        <v>14.540860309504001</v>
-      </c>
-      <c r="AI17" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="51">
-        <f t="shared" si="3"/>
         <v>2278.125</v>
       </c>
       <c r="AK17" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1822.5</v>
       </c>
       <c r="AL17" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1366.875</v>
       </c>
       <c r="AM17" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>17.915903999999998</v>
       </c>
     </row>
@@ -5569,155 +5593,155 @@
         <v>7</v>
       </c>
       <c r="B18" s="39">
-        <f>B17+B$5*$C$2^($A18)</f>
+        <f t="shared" si="0"/>
         <v>1649.9084800000001</v>
       </c>
       <c r="C18" s="26">
-        <f>C17+C$5*$C$2^($A18)</f>
+        <f t="shared" si="1"/>
         <v>1959.8901759999999</v>
       </c>
       <c r="D18" s="26">
-        <f>D17+D$5*$C$2^($A18)</f>
+        <f t="shared" si="2"/>
         <v>1649.9084800000001</v>
       </c>
       <c r="E18" s="40">
-        <f>E17+E$5*$C$2^($A18)</f>
+        <f t="shared" si="3"/>
         <v>1339.926784</v>
       </c>
       <c r="F18" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G18" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1366.875</v>
       </c>
       <c r="H18" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1025.15625</v>
       </c>
       <c r="I18" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1025.15625</v>
       </c>
       <c r="J18" s="45">
+        <f t="shared" si="9"/>
+        <v>11.641753802740478</v>
+      </c>
+      <c r="K18" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="32">
+        <f t="shared" si="8"/>
+        <v>1708.59375</v>
+      </c>
+      <c r="M18" s="32">
+        <f t="shared" si="8"/>
+        <v>1366.875</v>
+      </c>
+      <c r="N18" s="33">
+        <f t="shared" si="8"/>
+        <v>1025.15625</v>
+      </c>
+      <c r="O18" s="45">
+        <f t="shared" si="10"/>
+        <v>11.641753802740478</v>
+      </c>
+      <c r="P18" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="32">
+        <f t="shared" si="8"/>
+        <v>1366.875</v>
+      </c>
+      <c r="R18" s="32">
+        <f t="shared" si="8"/>
+        <v>1708.59375</v>
+      </c>
+      <c r="S18" s="33">
+        <f t="shared" si="8"/>
+        <v>1025.15625</v>
+      </c>
+      <c r="T18" s="45">
+        <f t="shared" si="11"/>
+        <v>11.641753802740478</v>
+      </c>
+      <c r="U18" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="32">
+        <f t="shared" si="8"/>
+        <v>1025.15625</v>
+      </c>
+      <c r="W18" s="32">
+        <f t="shared" si="8"/>
+        <v>1366.875</v>
+      </c>
+      <c r="X18" s="32">
+        <f t="shared" si="8"/>
+        <v>1708.59375</v>
+      </c>
+      <c r="Y18" s="45">
+        <f t="shared" si="12"/>
+        <v>11.641753802740478</v>
+      </c>
+      <c r="Z18" s="52">
+        <f t="shared" si="13"/>
+        <v>9572.562069798907</v>
+      </c>
+      <c r="AA18" s="19">
+        <f t="shared" si="14"/>
+        <v>9572.562069798907</v>
+      </c>
+      <c r="AB18" s="19">
         <f t="shared" si="5"/>
-        <v>11.641753802740478</v>
-      </c>
-      <c r="K18" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="32">
-        <f t="shared" si="4"/>
+        <v>9572.562069798907</v>
+      </c>
+      <c r="AC18" s="19">
+        <f t="shared" si="5"/>
+        <v>9572.562069798907</v>
+      </c>
+      <c r="AD18" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="51">
+        <f t="shared" si="6"/>
+        <v>3075.46875</v>
+      </c>
+      <c r="AF18" s="51">
+        <f t="shared" si="6"/>
+        <v>2392.03125</v>
+      </c>
+      <c r="AG18" s="57">
+        <f t="shared" si="6"/>
         <v>1708.59375</v>
       </c>
-      <c r="M18" s="32">
-        <f t="shared" si="4"/>
-        <v>1366.875</v>
-      </c>
-      <c r="N18" s="33">
-        <f t="shared" si="4"/>
-        <v>1025.15625</v>
-      </c>
-      <c r="O18" s="45">
-        <f t="shared" si="6"/>
-        <v>11.641753802740478</v>
-      </c>
-      <c r="P18" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="32">
-        <f t="shared" si="4"/>
-        <v>1366.875</v>
-      </c>
-      <c r="R18" s="32">
-        <f t="shared" si="4"/>
-        <v>1708.59375</v>
-      </c>
-      <c r="S18" s="33">
-        <f t="shared" si="4"/>
-        <v>1025.15625</v>
-      </c>
-      <c r="T18" s="45">
+      <c r="AH18" s="58">
+        <f t="shared" si="16"/>
+        <v>18.030666783784962</v>
+      </c>
+      <c r="AI18" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="51">
         <f t="shared" si="7"/>
-        <v>11.641753802740478</v>
-      </c>
-      <c r="U18" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V18" s="32">
-        <f t="shared" si="4"/>
-        <v>1025.15625</v>
-      </c>
-      <c r="W18" s="32">
-        <f t="shared" si="4"/>
-        <v>1366.875</v>
-      </c>
-      <c r="X18" s="32">
-        <f t="shared" si="4"/>
-        <v>1708.59375</v>
-      </c>
-      <c r="Y18" s="45">
-        <f t="shared" si="8"/>
-        <v>11.641753802740478</v>
-      </c>
-      <c r="Z18" s="52">
-        <f t="shared" si="9"/>
-        <v>9572.562069798907</v>
-      </c>
-      <c r="AA18" s="19">
-        <f t="shared" si="10"/>
-        <v>9572.562069798907</v>
-      </c>
-      <c r="AB18" s="19">
-        <f t="shared" si="1"/>
-        <v>9572.562069798907</v>
-      </c>
-      <c r="AC18" s="19">
-        <f t="shared" si="1"/>
-        <v>9572.562069798907</v>
-      </c>
-      <c r="AD18" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE18" s="51">
-        <f t="shared" si="2"/>
-        <v>3075.46875</v>
-      </c>
-      <c r="AF18" s="51">
-        <f t="shared" si="2"/>
-        <v>2392.03125</v>
-      </c>
-      <c r="AG18" s="57">
-        <f t="shared" si="2"/>
-        <v>1708.59375</v>
-      </c>
-      <c r="AH18" s="58">
-        <f t="shared" si="12"/>
-        <v>18.030666783784962</v>
-      </c>
-      <c r="AI18" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="51">
-        <f t="shared" si="3"/>
         <v>3417.1875</v>
       </c>
       <c r="AK18" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2733.75</v>
       </c>
       <c r="AL18" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2050.3125</v>
       </c>
       <c r="AM18" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>21.499084799999999</v>
       </c>
     </row>
@@ -5726,155 +5750,155 @@
         <v>8</v>
       </c>
       <c r="B19" s="39">
-        <f>B18+B$5*$C$2^($A19)</f>
+        <f t="shared" si="0"/>
         <v>2079.8901759999999</v>
       </c>
       <c r="C19" s="26">
-        <f>C18+C$5*$C$2^($A19)</f>
+        <f t="shared" si="1"/>
         <v>2475.8682111999997</v>
       </c>
       <c r="D19" s="26">
-        <f>D18+D$5*$C$2^($A19)</f>
+        <f t="shared" si="2"/>
         <v>2079.8901759999999</v>
       </c>
       <c r="E19" s="40">
-        <f>E18+E$5*$C$2^($A19)</f>
+        <f t="shared" si="3"/>
         <v>1683.9121408000001</v>
       </c>
       <c r="F19" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G19" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2050.3125</v>
       </c>
       <c r="H19" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1537.734375</v>
       </c>
       <c r="I19" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1537.734375</v>
       </c>
       <c r="J19" s="45">
+        <f t="shared" si="9"/>
+        <v>16.531290399891478</v>
+      </c>
+      <c r="K19" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="32">
+        <f t="shared" si="8"/>
+        <v>2562.890625</v>
+      </c>
+      <c r="M19" s="32">
+        <f t="shared" si="8"/>
+        <v>2050.3125</v>
+      </c>
+      <c r="N19" s="33">
+        <f t="shared" si="8"/>
+        <v>1537.734375</v>
+      </c>
+      <c r="O19" s="45">
+        <f t="shared" si="10"/>
+        <v>16.531290399891478</v>
+      </c>
+      <c r="P19" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="32">
+        <f t="shared" si="8"/>
+        <v>2050.3125</v>
+      </c>
+      <c r="R19" s="32">
+        <f t="shared" si="8"/>
+        <v>2562.890625</v>
+      </c>
+      <c r="S19" s="33">
+        <f t="shared" si="8"/>
+        <v>1537.734375</v>
+      </c>
+      <c r="T19" s="45">
+        <f t="shared" si="11"/>
+        <v>16.531290399891478</v>
+      </c>
+      <c r="U19" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="32">
+        <f t="shared" si="8"/>
+        <v>1537.734375</v>
+      </c>
+      <c r="W19" s="32">
+        <f t="shared" si="8"/>
+        <v>2050.3125</v>
+      </c>
+      <c r="X19" s="32">
+        <f t="shared" si="8"/>
+        <v>2562.890625</v>
+      </c>
+      <c r="Y19" s="45">
+        <f t="shared" si="12"/>
+        <v>16.531290399891478</v>
+      </c>
+      <c r="Z19" s="52">
+        <f t="shared" si="13"/>
+        <v>15699.001794470207</v>
+      </c>
+      <c r="AA19" s="19">
+        <f t="shared" si="14"/>
+        <v>15699.001794470207</v>
+      </c>
+      <c r="AB19" s="19">
         <f t="shared" si="5"/>
-        <v>16.531290399891478</v>
-      </c>
-      <c r="K19" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="32">
-        <f t="shared" si="4"/>
+        <v>15699.001794470207</v>
+      </c>
+      <c r="AC19" s="19">
+        <f t="shared" si="5"/>
+        <v>15699.001794470207</v>
+      </c>
+      <c r="AD19" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE19" s="51">
+        <f t="shared" si="6"/>
+        <v>4613.203125</v>
+      </c>
+      <c r="AF19" s="51">
+        <f t="shared" si="6"/>
+        <v>3588.046875</v>
+      </c>
+      <c r="AG19" s="57">
+        <f t="shared" si="6"/>
         <v>2562.890625</v>
       </c>
-      <c r="M19" s="32">
-        <f t="shared" si="4"/>
-        <v>2050.3125</v>
-      </c>
-      <c r="N19" s="33">
-        <f t="shared" si="4"/>
-        <v>1537.734375</v>
-      </c>
-      <c r="O19" s="45">
-        <f t="shared" si="6"/>
-        <v>16.531290399891478</v>
-      </c>
-      <c r="P19" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="32">
-        <f t="shared" si="4"/>
-        <v>2050.3125</v>
-      </c>
-      <c r="R19" s="32">
-        <f t="shared" si="4"/>
-        <v>2562.890625</v>
-      </c>
-      <c r="S19" s="33">
-        <f t="shared" si="4"/>
-        <v>1537.734375</v>
-      </c>
-      <c r="T19" s="45">
+      <c r="AH19" s="58">
+        <f t="shared" si="16"/>
+        <v>22.358026811893353</v>
+      </c>
+      <c r="AI19" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="51">
         <f t="shared" si="7"/>
-        <v>16.531290399891478</v>
-      </c>
-      <c r="U19" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="32">
-        <f t="shared" si="4"/>
-        <v>1537.734375</v>
-      </c>
-      <c r="W19" s="32">
-        <f t="shared" si="4"/>
-        <v>2050.3125</v>
-      </c>
-      <c r="X19" s="32">
-        <f t="shared" si="4"/>
-        <v>2562.890625</v>
-      </c>
-      <c r="Y19" s="45">
-        <f t="shared" si="8"/>
-        <v>16.531290399891478</v>
-      </c>
-      <c r="Z19" s="52">
-        <f t="shared" si="9"/>
-        <v>15699.001794470207</v>
-      </c>
-      <c r="AA19" s="19">
-        <f t="shared" si="10"/>
-        <v>15699.001794470207</v>
-      </c>
-      <c r="AB19" s="19">
-        <f t="shared" si="1"/>
-        <v>15699.001794470207</v>
-      </c>
-      <c r="AC19" s="19">
-        <f t="shared" si="1"/>
-        <v>15699.001794470207</v>
-      </c>
-      <c r="AD19" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE19" s="51">
-        <f t="shared" si="2"/>
-        <v>4613.203125</v>
-      </c>
-      <c r="AF19" s="51">
-        <f t="shared" si="2"/>
-        <v>3588.046875</v>
-      </c>
-      <c r="AG19" s="57">
-        <f t="shared" si="2"/>
-        <v>2562.890625</v>
-      </c>
-      <c r="AH19" s="58">
-        <f t="shared" si="12"/>
-        <v>22.358026811893353</v>
-      </c>
-      <c r="AI19" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="51">
-        <f t="shared" si="3"/>
         <v>5125.78125</v>
       </c>
       <c r="AK19" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4100.625</v>
       </c>
       <c r="AL19" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3075.46875</v>
       </c>
       <c r="AM19" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>25.798901759999996</v>
       </c>
     </row>
@@ -5883,155 +5907,155 @@
         <v>9</v>
       </c>
       <c r="B20" s="39">
-        <f>B19+B$5*$C$2^($A20)</f>
+        <f t="shared" si="0"/>
         <v>2595.8682111999997</v>
       </c>
       <c r="C20" s="26">
-        <f>C19+C$5*$C$2^($A20)</f>
+        <f t="shared" si="1"/>
         <v>3095.0418534399996</v>
       </c>
       <c r="D20" s="26">
-        <f>D19+D$5*$C$2^($A20)</f>
+        <f t="shared" si="2"/>
         <v>2595.8682111999997</v>
       </c>
       <c r="E20" s="40">
-        <f>E19+E$5*$C$2^($A20)</f>
+        <f t="shared" si="3"/>
         <v>2096.6945689600002</v>
       </c>
       <c r="F20" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G20" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3075.46875</v>
       </c>
       <c r="H20" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2306.6015625</v>
       </c>
       <c r="I20" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2306.6015625</v>
       </c>
       <c r="J20" s="45">
+        <f t="shared" si="9"/>
+        <v>23.4744323678459</v>
+      </c>
+      <c r="K20" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="32">
+        <f t="shared" si="8"/>
+        <v>3844.3359375</v>
+      </c>
+      <c r="M20" s="32">
+        <f t="shared" si="8"/>
+        <v>3075.46875</v>
+      </c>
+      <c r="N20" s="33">
+        <f t="shared" si="8"/>
+        <v>2306.6015625</v>
+      </c>
+      <c r="O20" s="45">
+        <f t="shared" si="10"/>
+        <v>23.4744323678459</v>
+      </c>
+      <c r="P20" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="32">
+        <f t="shared" si="8"/>
+        <v>3075.46875</v>
+      </c>
+      <c r="R20" s="32">
+        <f t="shared" si="8"/>
+        <v>3844.3359375</v>
+      </c>
+      <c r="S20" s="33">
+        <f t="shared" si="8"/>
+        <v>2306.6015625</v>
+      </c>
+      <c r="T20" s="45">
+        <f t="shared" si="11"/>
+        <v>23.4744323678459</v>
+      </c>
+      <c r="U20" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="32">
+        <f t="shared" si="8"/>
+        <v>2306.6015625</v>
+      </c>
+      <c r="W20" s="32">
+        <f t="shared" si="8"/>
+        <v>3075.46875</v>
+      </c>
+      <c r="X20" s="32">
+        <f t="shared" si="8"/>
+        <v>3844.3359375</v>
+      </c>
+      <c r="Y20" s="45">
+        <f t="shared" si="12"/>
+        <v>23.4744323678459</v>
+      </c>
+      <c r="Z20" s="52">
+        <f t="shared" si="13"/>
+        <v>25746.362942931137</v>
+      </c>
+      <c r="AA20" s="19">
+        <f t="shared" si="14"/>
+        <v>25746.362942931137</v>
+      </c>
+      <c r="AB20" s="19">
         <f t="shared" si="5"/>
-        <v>23.4744323678459</v>
-      </c>
-      <c r="K20" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="32">
-        <f t="shared" si="4"/>
+        <v>25746.362942931137</v>
+      </c>
+      <c r="AC20" s="19">
+        <f t="shared" si="5"/>
+        <v>25746.362942931137</v>
+      </c>
+      <c r="AD20" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE20" s="51">
+        <f t="shared" si="6"/>
+        <v>6919.8046875</v>
+      </c>
+      <c r="AF20" s="51">
+        <f t="shared" si="6"/>
+        <v>5382.0703125</v>
+      </c>
+      <c r="AG20" s="57">
+        <f t="shared" si="6"/>
         <v>3844.3359375</v>
       </c>
-      <c r="M20" s="32">
-        <f t="shared" si="4"/>
-        <v>3075.46875</v>
-      </c>
-      <c r="N20" s="33">
-        <f t="shared" si="4"/>
-        <v>2306.6015625</v>
-      </c>
-      <c r="O20" s="45">
-        <f t="shared" si="6"/>
-        <v>23.4744323678459</v>
-      </c>
-      <c r="P20" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="32">
-        <f t="shared" si="4"/>
-        <v>3075.46875</v>
-      </c>
-      <c r="R20" s="32">
-        <f t="shared" si="4"/>
-        <v>3844.3359375</v>
-      </c>
-      <c r="S20" s="33">
-        <f t="shared" si="4"/>
-        <v>2306.6015625</v>
-      </c>
-      <c r="T20" s="45">
+      <c r="AH20" s="58">
+        <f t="shared" si="16"/>
+        <v>27.723953246747758</v>
+      </c>
+      <c r="AI20" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="51">
         <f t="shared" si="7"/>
-        <v>23.4744323678459</v>
-      </c>
-      <c r="U20" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V20" s="32">
-        <f t="shared" si="4"/>
-        <v>2306.6015625</v>
-      </c>
-      <c r="W20" s="32">
-        <f t="shared" si="4"/>
-        <v>3075.46875</v>
-      </c>
-      <c r="X20" s="32">
-        <f t="shared" si="4"/>
-        <v>3844.3359375</v>
-      </c>
-      <c r="Y20" s="45">
-        <f t="shared" si="8"/>
-        <v>23.4744323678459</v>
-      </c>
-      <c r="Z20" s="52">
-        <f t="shared" si="9"/>
-        <v>25746.362942931137</v>
-      </c>
-      <c r="AA20" s="19">
-        <f t="shared" si="10"/>
-        <v>25746.362942931137</v>
-      </c>
-      <c r="AB20" s="19">
-        <f t="shared" si="1"/>
-        <v>25746.362942931137</v>
-      </c>
-      <c r="AC20" s="19">
-        <f t="shared" si="1"/>
-        <v>25746.362942931137</v>
-      </c>
-      <c r="AD20" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE20" s="51">
-        <f t="shared" si="2"/>
-        <v>6919.8046875</v>
-      </c>
-      <c r="AF20" s="51">
-        <f t="shared" si="2"/>
-        <v>5382.0703125</v>
-      </c>
-      <c r="AG20" s="57">
-        <f t="shared" si="2"/>
-        <v>3844.3359375</v>
-      </c>
-      <c r="AH20" s="58">
-        <f t="shared" si="12"/>
-        <v>27.723953246747758</v>
-      </c>
-      <c r="AI20" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="51">
-        <f t="shared" si="3"/>
         <v>7688.671875</v>
       </c>
       <c r="AK20" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6150.9375</v>
       </c>
       <c r="AL20" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4613.203125</v>
       </c>
       <c r="AM20" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>30.958682111999998</v>
       </c>
     </row>
@@ -6040,155 +6064,155 @@
         <v>10</v>
       </c>
       <c r="B21" s="39">
-        <f>B20+B$5*$C$2^($A21)</f>
+        <f t="shared" si="0"/>
         <v>3215.0418534399996</v>
       </c>
       <c r="C21" s="26">
-        <f>C20+C$5*$C$2^($A21)</f>
+        <f t="shared" si="1"/>
         <v>3838.0502241279996</v>
       </c>
       <c r="D21" s="26">
-        <f>D20+D$5*$C$2^($A21)</f>
+        <f t="shared" si="2"/>
         <v>3215.0418534399996</v>
       </c>
       <c r="E21" s="40">
-        <f>E20+E$5*$C$2^($A21)</f>
+        <f t="shared" si="3"/>
         <v>2592.0334827520001</v>
       </c>
       <c r="F21" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G21" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4613.203125</v>
       </c>
       <c r="H21" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3459.90234375</v>
       </c>
       <c r="I21" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3459.90234375</v>
       </c>
       <c r="J21" s="45">
+        <f t="shared" si="9"/>
+        <v>33.333693962341179</v>
+      </c>
+      <c r="K21" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="32">
+        <f t="shared" si="8"/>
+        <v>5766.50390625</v>
+      </c>
+      <c r="M21" s="32">
+        <f t="shared" si="8"/>
+        <v>4613.203125</v>
+      </c>
+      <c r="N21" s="33">
+        <f t="shared" si="8"/>
+        <v>3459.90234375</v>
+      </c>
+      <c r="O21" s="45">
+        <f t="shared" si="10"/>
+        <v>33.333693962341179</v>
+      </c>
+      <c r="P21" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="32">
+        <f t="shared" si="8"/>
+        <v>4613.203125</v>
+      </c>
+      <c r="R21" s="32">
+        <f t="shared" si="8"/>
+        <v>5766.50390625</v>
+      </c>
+      <c r="S21" s="33">
+        <f t="shared" si="8"/>
+        <v>3459.90234375</v>
+      </c>
+      <c r="T21" s="45">
+        <f t="shared" si="11"/>
+        <v>33.333693962341179</v>
+      </c>
+      <c r="U21" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V21" s="32">
+        <f t="shared" si="8"/>
+        <v>3459.90234375</v>
+      </c>
+      <c r="W21" s="32">
+        <f t="shared" si="8"/>
+        <v>4613.203125</v>
+      </c>
+      <c r="X21" s="32">
+        <f t="shared" si="8"/>
+        <v>5766.50390625</v>
+      </c>
+      <c r="Y21" s="45">
+        <f t="shared" si="12"/>
+        <v>33.333693962341179</v>
+      </c>
+      <c r="Z21" s="52">
+        <f t="shared" si="13"/>
+        <v>42224.035226407061</v>
+      </c>
+      <c r="AA21" s="19">
+        <f t="shared" si="14"/>
+        <v>42224.035226407061</v>
+      </c>
+      <c r="AB21" s="19">
         <f t="shared" si="5"/>
-        <v>33.333693962341179</v>
-      </c>
-      <c r="K21" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="32">
-        <f t="shared" si="4"/>
+        <v>42224.035226407061</v>
+      </c>
+      <c r="AC21" s="19">
+        <f t="shared" si="5"/>
+        <v>42224.035226407061</v>
+      </c>
+      <c r="AD21" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="51">
+        <f t="shared" si="6"/>
+        <v>10379.70703125</v>
+      </c>
+      <c r="AF21" s="51">
+        <f t="shared" si="6"/>
+        <v>8073.10546875</v>
+      </c>
+      <c r="AG21" s="57">
+        <f t="shared" si="6"/>
         <v>5766.50390625</v>
       </c>
-      <c r="M21" s="32">
-        <f t="shared" si="4"/>
-        <v>4613.203125</v>
-      </c>
-      <c r="N21" s="33">
-        <f t="shared" si="4"/>
-        <v>3459.90234375</v>
-      </c>
-      <c r="O21" s="45">
-        <f t="shared" si="6"/>
-        <v>33.333693962341179</v>
-      </c>
-      <c r="P21" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="32">
-        <f t="shared" si="4"/>
-        <v>4613.203125</v>
-      </c>
-      <c r="R21" s="32">
-        <f t="shared" si="4"/>
-        <v>5766.50390625</v>
-      </c>
-      <c r="S21" s="33">
-        <f t="shared" si="4"/>
-        <v>3459.90234375</v>
-      </c>
-      <c r="T21" s="45">
+      <c r="AH21" s="58">
+        <f t="shared" si="16"/>
+        <v>34.377702025967224</v>
+      </c>
+      <c r="AI21" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="51">
         <f t="shared" si="7"/>
-        <v>33.333693962341179</v>
-      </c>
-      <c r="U21" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V21" s="32">
-        <f t="shared" si="4"/>
-        <v>3459.90234375</v>
-      </c>
-      <c r="W21" s="32">
-        <f t="shared" si="4"/>
-        <v>4613.203125</v>
-      </c>
-      <c r="X21" s="32">
-        <f t="shared" si="4"/>
-        <v>5766.50390625</v>
-      </c>
-      <c r="Y21" s="45">
-        <f t="shared" si="8"/>
-        <v>33.333693962341179</v>
-      </c>
-      <c r="Z21" s="52">
-        <f t="shared" si="9"/>
-        <v>42224.035226407061</v>
-      </c>
-      <c r="AA21" s="19">
-        <f t="shared" si="10"/>
-        <v>42224.035226407061</v>
-      </c>
-      <c r="AB21" s="19">
-        <f t="shared" si="1"/>
-        <v>42224.035226407061</v>
-      </c>
-      <c r="AC21" s="19">
-        <f t="shared" si="1"/>
-        <v>42224.035226407061</v>
-      </c>
-      <c r="AD21" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE21" s="51">
-        <f t="shared" si="2"/>
-        <v>10379.70703125</v>
-      </c>
-      <c r="AF21" s="51">
-        <f t="shared" si="2"/>
-        <v>8073.10546875</v>
-      </c>
-      <c r="AG21" s="57">
-        <f t="shared" si="2"/>
-        <v>5766.50390625</v>
-      </c>
-      <c r="AH21" s="58">
-        <f t="shared" si="12"/>
-        <v>34.377702025967224</v>
-      </c>
-      <c r="AI21" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ21" s="51">
-        <f t="shared" si="3"/>
         <v>11533.0078125</v>
       </c>
       <c r="AK21" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9226.40625</v>
       </c>
       <c r="AL21" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6919.8046875</v>
       </c>
       <c r="AM21" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>37.150418534399996</v>
       </c>
     </row>
@@ -6197,155 +6221,155 @@
         <v>11</v>
       </c>
       <c r="B22" s="39">
-        <f>B21+B$5*$C$2^($A22)</f>
+        <f t="shared" si="0"/>
         <v>3958.0502241279996</v>
       </c>
       <c r="C22" s="26">
-        <f>C21+C$5*$C$2^($A22)</f>
+        <f t="shared" si="1"/>
         <v>4729.6602689535994</v>
       </c>
       <c r="D22" s="26">
-        <f>D21+D$5*$C$2^($A22)</f>
+        <f t="shared" si="2"/>
         <v>3958.0502241279996</v>
       </c>
       <c r="E22" s="40">
-        <f>E21+E$5*$C$2^($A22)</f>
+        <f t="shared" si="3"/>
         <v>3186.4401793023999</v>
       </c>
       <c r="F22" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G22" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6919.8046875</v>
       </c>
       <c r="H22" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5189.853515625</v>
       </c>
       <c r="I22" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5189.853515625</v>
       </c>
       <c r="J22" s="45">
+        <f t="shared" si="9"/>
+        <v>47.333845426524469</v>
+      </c>
+      <c r="K22" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="32">
+        <f t="shared" si="8"/>
+        <v>8649.755859375</v>
+      </c>
+      <c r="M22" s="32">
+        <f t="shared" si="8"/>
+        <v>6919.8046875</v>
+      </c>
+      <c r="N22" s="33">
+        <f t="shared" si="8"/>
+        <v>5189.853515625</v>
+      </c>
+      <c r="O22" s="45">
+        <f t="shared" si="10"/>
+        <v>47.333845426524469</v>
+      </c>
+      <c r="P22" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="32">
+        <f t="shared" si="8"/>
+        <v>6919.8046875</v>
+      </c>
+      <c r="R22" s="32">
+        <f t="shared" si="8"/>
+        <v>8649.755859375</v>
+      </c>
+      <c r="S22" s="33">
+        <f t="shared" si="8"/>
+        <v>5189.853515625</v>
+      </c>
+      <c r="T22" s="45">
+        <f t="shared" si="11"/>
+        <v>47.333845426524469</v>
+      </c>
+      <c r="U22" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="32">
+        <f t="shared" si="8"/>
+        <v>5189.853515625</v>
+      </c>
+      <c r="W22" s="32">
+        <f t="shared" si="8"/>
+        <v>6919.8046875</v>
+      </c>
+      <c r="X22" s="32">
+        <f t="shared" si="8"/>
+        <v>8649.755859375</v>
+      </c>
+      <c r="Y22" s="45">
+        <f t="shared" si="12"/>
+        <v>47.333845426524469</v>
+      </c>
+      <c r="Z22" s="52">
+        <f t="shared" si="13"/>
+        <v>69247.417771307562</v>
+      </c>
+      <c r="AA22" s="19">
+        <f t="shared" si="14"/>
+        <v>69247.417771307562</v>
+      </c>
+      <c r="AB22" s="19">
         <f t="shared" si="5"/>
-        <v>47.333845426524469</v>
-      </c>
-      <c r="K22" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="32">
-        <f t="shared" si="4"/>
+        <v>69247.417771307562</v>
+      </c>
+      <c r="AC22" s="19">
+        <f t="shared" si="5"/>
+        <v>69247.417771307562</v>
+      </c>
+      <c r="AD22" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE22" s="51">
+        <f t="shared" si="6"/>
+        <v>15569.560546875</v>
+      </c>
+      <c r="AF22" s="51">
+        <f t="shared" si="6"/>
+        <v>12109.658203125</v>
+      </c>
+      <c r="AG22" s="57">
+        <f t="shared" si="6"/>
         <v>8649.755859375</v>
       </c>
-      <c r="M22" s="32">
-        <f t="shared" si="4"/>
-        <v>6919.8046875</v>
-      </c>
-      <c r="N22" s="33">
-        <f t="shared" si="4"/>
-        <v>5189.853515625</v>
-      </c>
-      <c r="O22" s="45">
-        <f t="shared" si="6"/>
-        <v>47.333845426524469</v>
-      </c>
-      <c r="P22" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="32">
-        <f t="shared" si="4"/>
-        <v>6919.8046875</v>
-      </c>
-      <c r="R22" s="32">
-        <f t="shared" si="4"/>
-        <v>8649.755859375</v>
-      </c>
-      <c r="S22" s="33">
-        <f t="shared" si="4"/>
-        <v>5189.853515625</v>
-      </c>
-      <c r="T22" s="45">
+      <c r="AH22" s="58">
+        <f t="shared" si="16"/>
+        <v>42.628350512199354</v>
+      </c>
+      <c r="AI22" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="51">
         <f t="shared" si="7"/>
-        <v>47.333845426524469</v>
-      </c>
-      <c r="U22" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V22" s="32">
-        <f t="shared" si="4"/>
-        <v>5189.853515625</v>
-      </c>
-      <c r="W22" s="32">
-        <f t="shared" si="4"/>
-        <v>6919.8046875</v>
-      </c>
-      <c r="X22" s="32">
-        <f t="shared" si="4"/>
-        <v>8649.755859375</v>
-      </c>
-      <c r="Y22" s="45">
-        <f t="shared" si="8"/>
-        <v>47.333845426524469</v>
-      </c>
-      <c r="Z22" s="52">
-        <f t="shared" si="9"/>
-        <v>69247.417771307562</v>
-      </c>
-      <c r="AA22" s="19">
-        <f t="shared" si="10"/>
-        <v>69247.417771307562</v>
-      </c>
-      <c r="AB22" s="19">
-        <f t="shared" si="1"/>
-        <v>69247.417771307562</v>
-      </c>
-      <c r="AC22" s="19">
-        <f t="shared" si="1"/>
-        <v>69247.417771307562</v>
-      </c>
-      <c r="AD22" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE22" s="51">
-        <f t="shared" si="2"/>
-        <v>15569.560546875</v>
-      </c>
-      <c r="AF22" s="51">
-        <f t="shared" si="2"/>
-        <v>12109.658203125</v>
-      </c>
-      <c r="AG22" s="57">
-        <f t="shared" si="2"/>
-        <v>8649.755859375</v>
-      </c>
-      <c r="AH22" s="58">
-        <f t="shared" si="12"/>
-        <v>42.628350512199354</v>
-      </c>
-      <c r="AI22" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="51">
-        <f t="shared" si="3"/>
         <v>17299.51171875</v>
       </c>
       <c r="AK22" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>13839.609375</v>
       </c>
       <c r="AL22" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>10379.70703125</v>
       </c>
       <c r="AM22" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>44.580502241279994</v>
       </c>
     </row>
@@ -6354,155 +6378,155 @@
         <v>12</v>
       </c>
       <c r="B23" s="39">
-        <f>B22+B$5*$C$2^($A23)</f>
+        <f t="shared" si="0"/>
         <v>4849.6602689535994</v>
       </c>
       <c r="C23" s="26">
-        <f>C22+C$5*$C$2^($A23)</f>
+        <f t="shared" si="1"/>
         <v>5799.5923227443191</v>
       </c>
       <c r="D23" s="26">
-        <f>D22+D$5*$C$2^($A23)</f>
+        <f t="shared" si="2"/>
         <v>4849.6602689535994</v>
       </c>
       <c r="E23" s="40">
-        <f>E22+E$5*$C$2^($A23)</f>
+        <f t="shared" si="3"/>
         <v>3899.7282151628797</v>
       </c>
       <c r="F23" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G23" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>10379.70703125</v>
       </c>
       <c r="H23" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7784.7802734375</v>
       </c>
       <c r="I23" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7784.7802734375</v>
       </c>
       <c r="J23" s="45">
+        <f t="shared" si="9"/>
+        <v>67.214060505664747</v>
+      </c>
+      <c r="K23" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="32">
+        <f t="shared" si="8"/>
+        <v>12974.6337890625</v>
+      </c>
+      <c r="M23" s="32">
+        <f t="shared" si="8"/>
+        <v>10379.70703125</v>
+      </c>
+      <c r="N23" s="33">
+        <f t="shared" si="8"/>
+        <v>7784.7802734375</v>
+      </c>
+      <c r="O23" s="45">
+        <f t="shared" si="10"/>
+        <v>67.214060505664747</v>
+      </c>
+      <c r="P23" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="32">
+        <f t="shared" si="8"/>
+        <v>10379.70703125</v>
+      </c>
+      <c r="R23" s="32">
+        <f t="shared" si="8"/>
+        <v>12974.6337890625</v>
+      </c>
+      <c r="S23" s="33">
+        <f t="shared" si="8"/>
+        <v>7784.7802734375</v>
+      </c>
+      <c r="T23" s="45">
+        <f t="shared" si="11"/>
+        <v>67.214060505664747</v>
+      </c>
+      <c r="U23" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="32">
+        <f t="shared" si="8"/>
+        <v>7784.7802734375</v>
+      </c>
+      <c r="W23" s="32">
+        <f t="shared" si="8"/>
+        <v>10379.70703125</v>
+      </c>
+      <c r="X23" s="32">
+        <f t="shared" si="8"/>
+        <v>12974.6337890625</v>
+      </c>
+      <c r="Y23" s="45">
+        <f t="shared" si="12"/>
+        <v>67.214060505664747</v>
+      </c>
+      <c r="Z23" s="52">
+        <f t="shared" si="13"/>
+        <v>113565.76514494441</v>
+      </c>
+      <c r="AA23" s="19">
+        <f t="shared" si="14"/>
+        <v>113565.76514494441</v>
+      </c>
+      <c r="AB23" s="19">
         <f t="shared" si="5"/>
-        <v>67.214060505664747</v>
-      </c>
-      <c r="K23" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="32">
-        <f t="shared" si="4"/>
+        <v>113565.76514494441</v>
+      </c>
+      <c r="AC23" s="19">
+        <f t="shared" si="5"/>
+        <v>113565.76514494441</v>
+      </c>
+      <c r="AD23" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE23" s="51">
+        <f t="shared" si="6"/>
+        <v>23354.3408203125</v>
+      </c>
+      <c r="AF23" s="51">
+        <f t="shared" si="6"/>
+        <v>18164.4873046875</v>
+      </c>
+      <c r="AG23" s="57">
+        <f t="shared" si="6"/>
         <v>12974.6337890625</v>
       </c>
-      <c r="M23" s="32">
-        <f t="shared" si="4"/>
-        <v>10379.70703125</v>
-      </c>
-      <c r="N23" s="33">
-        <f t="shared" si="4"/>
-        <v>7784.7802734375</v>
-      </c>
-      <c r="O23" s="45">
-        <f t="shared" si="6"/>
-        <v>67.214060505664747</v>
-      </c>
-      <c r="P23" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="32">
-        <f t="shared" si="4"/>
-        <v>10379.70703125</v>
-      </c>
-      <c r="R23" s="32">
-        <f t="shared" si="4"/>
-        <v>12974.6337890625</v>
-      </c>
-      <c r="S23" s="33">
-        <f t="shared" si="4"/>
-        <v>7784.7802734375</v>
-      </c>
-      <c r="T23" s="45">
+      <c r="AH23" s="58">
+        <f t="shared" si="16"/>
+        <v>52.859154635127204</v>
+      </c>
+      <c r="AI23" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="51">
         <f t="shared" si="7"/>
-        <v>67.214060505664747</v>
-      </c>
-      <c r="U23" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V23" s="32">
-        <f t="shared" si="4"/>
-        <v>7784.7802734375</v>
-      </c>
-      <c r="W23" s="32">
-        <f t="shared" si="4"/>
-        <v>10379.70703125</v>
-      </c>
-      <c r="X23" s="32">
-        <f t="shared" si="4"/>
-        <v>12974.6337890625</v>
-      </c>
-      <c r="Y23" s="45">
-        <f t="shared" si="8"/>
-        <v>67.214060505664747</v>
-      </c>
-      <c r="Z23" s="52">
-        <f t="shared" si="9"/>
-        <v>113565.76514494441</v>
-      </c>
-      <c r="AA23" s="19">
-        <f t="shared" si="10"/>
-        <v>113565.76514494441</v>
-      </c>
-      <c r="AB23" s="19">
-        <f t="shared" si="1"/>
-        <v>113565.76514494441</v>
-      </c>
-      <c r="AC23" s="19">
-        <f t="shared" si="1"/>
-        <v>113565.76514494441</v>
-      </c>
-      <c r="AD23" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE23" s="51">
-        <f t="shared" si="2"/>
-        <v>23354.3408203125</v>
-      </c>
-      <c r="AF23" s="51">
-        <f t="shared" si="2"/>
-        <v>18164.4873046875</v>
-      </c>
-      <c r="AG23" s="57">
-        <f t="shared" si="2"/>
-        <v>12974.6337890625</v>
-      </c>
-      <c r="AH23" s="58">
-        <f t="shared" si="12"/>
-        <v>52.859154635127204</v>
-      </c>
-      <c r="AI23" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="51">
-        <f t="shared" si="3"/>
         <v>25949.267578125</v>
       </c>
       <c r="AK23" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>20759.4140625</v>
       </c>
       <c r="AL23" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>15569.560546875</v>
       </c>
       <c r="AM23" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>53.49660268953599</v>
       </c>
     </row>
@@ -6511,155 +6535,155 @@
         <v>13</v>
       </c>
       <c r="B24" s="39">
-        <f>B23+B$5*$C$2^($A24)</f>
+        <f t="shared" si="0"/>
         <v>5919.5923227443191</v>
       </c>
       <c r="C24" s="26">
-        <f>C23+C$5*$C$2^($A24)</f>
+        <f t="shared" si="1"/>
         <v>7083.5107872931831</v>
       </c>
       <c r="D24" s="26">
-        <f>D23+D$5*$C$2^($A24)</f>
+        <f t="shared" si="2"/>
         <v>5919.5923227443191</v>
       </c>
       <c r="E24" s="40">
-        <f>E23+E$5*$C$2^($A24)</f>
+        <f t="shared" si="3"/>
         <v>4755.673858195456</v>
       </c>
       <c r="F24" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G24" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>15569.560546875</v>
       </c>
       <c r="H24" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11677.17041015625</v>
       </c>
       <c r="I24" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11677.17041015625</v>
       </c>
       <c r="J24" s="45">
+        <f t="shared" si="9"/>
+        <v>95.443965918043929</v>
+      </c>
+      <c r="K24" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="32">
+        <f t="shared" si="8"/>
+        <v>19461.95068359375</v>
+      </c>
+      <c r="M24" s="32">
+        <f t="shared" si="8"/>
+        <v>15569.560546875</v>
+      </c>
+      <c r="N24" s="33">
+        <f t="shared" si="8"/>
+        <v>11677.17041015625</v>
+      </c>
+      <c r="O24" s="45">
+        <f t="shared" si="10"/>
+        <v>95.443965918043929</v>
+      </c>
+      <c r="P24" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="32">
+        <f t="shared" si="8"/>
+        <v>15569.560546875</v>
+      </c>
+      <c r="R24" s="32">
+        <f t="shared" si="8"/>
+        <v>19461.95068359375</v>
+      </c>
+      <c r="S24" s="33">
+        <f t="shared" si="8"/>
+        <v>11677.17041015625</v>
+      </c>
+      <c r="T24" s="45">
+        <f t="shared" si="11"/>
+        <v>95.443965918043929</v>
+      </c>
+      <c r="U24" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="32">
+        <f t="shared" si="8"/>
+        <v>11677.17041015625</v>
+      </c>
+      <c r="W24" s="32">
+        <f t="shared" si="8"/>
+        <v>15569.560546875</v>
+      </c>
+      <c r="X24" s="32">
+        <f t="shared" si="8"/>
+        <v>19461.95068359375</v>
+      </c>
+      <c r="Y24" s="45">
+        <f t="shared" si="12"/>
+        <v>95.443965918043929</v>
+      </c>
+      <c r="Z24" s="52">
+        <f t="shared" si="13"/>
+        <v>186247.85483770882</v>
+      </c>
+      <c r="AA24" s="19">
+        <f t="shared" si="14"/>
+        <v>186247.85483770882</v>
+      </c>
+      <c r="AB24" s="19">
         <f t="shared" si="5"/>
-        <v>95.443965918043929</v>
-      </c>
-      <c r="K24" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="32">
-        <f t="shared" si="4"/>
+        <v>186247.85483770882</v>
+      </c>
+      <c r="AC24" s="19">
+        <f t="shared" si="5"/>
+        <v>186247.85483770882</v>
+      </c>
+      <c r="AD24" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="51">
+        <f t="shared" si="6"/>
+        <v>35031.51123046875</v>
+      </c>
+      <c r="AF24" s="51">
+        <f t="shared" si="6"/>
+        <v>27246.73095703125</v>
+      </c>
+      <c r="AG24" s="57">
+        <f t="shared" si="6"/>
         <v>19461.95068359375</v>
       </c>
-      <c r="M24" s="32">
-        <f t="shared" si="4"/>
-        <v>15569.560546875</v>
-      </c>
-      <c r="N24" s="33">
-        <f t="shared" si="4"/>
-        <v>11677.17041015625</v>
-      </c>
-      <c r="O24" s="45">
-        <f t="shared" si="6"/>
-        <v>95.443965918043929</v>
-      </c>
-      <c r="P24" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="32">
-        <f t="shared" si="4"/>
-        <v>15569.560546875</v>
-      </c>
-      <c r="R24" s="32">
-        <f t="shared" si="4"/>
-        <v>19461.95068359375</v>
-      </c>
-      <c r="S24" s="33">
-        <f t="shared" si="4"/>
-        <v>11677.17041015625</v>
-      </c>
-      <c r="T24" s="45">
+      <c r="AH24" s="58">
+        <f t="shared" si="16"/>
+        <v>65.545351747557731</v>
+      </c>
+      <c r="AI24" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="51">
         <f t="shared" si="7"/>
-        <v>95.443965918043929</v>
-      </c>
-      <c r="U24" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V24" s="32">
-        <f t="shared" si="4"/>
-        <v>11677.17041015625</v>
-      </c>
-      <c r="W24" s="32">
-        <f t="shared" si="4"/>
-        <v>15569.560546875</v>
-      </c>
-      <c r="X24" s="32">
-        <f t="shared" si="4"/>
-        <v>19461.95068359375</v>
-      </c>
-      <c r="Y24" s="45">
-        <f t="shared" si="8"/>
-        <v>95.443965918043929</v>
-      </c>
-      <c r="Z24" s="52">
-        <f t="shared" si="9"/>
-        <v>186247.85483770882</v>
-      </c>
-      <c r="AA24" s="19">
-        <f t="shared" si="10"/>
-        <v>186247.85483770882</v>
-      </c>
-      <c r="AB24" s="19">
-        <f t="shared" si="1"/>
-        <v>186247.85483770882</v>
-      </c>
-      <c r="AC24" s="19">
-        <f t="shared" si="1"/>
-        <v>186247.85483770882</v>
-      </c>
-      <c r="AD24" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE24" s="51">
-        <f t="shared" si="2"/>
-        <v>35031.51123046875</v>
-      </c>
-      <c r="AF24" s="51">
-        <f t="shared" si="2"/>
-        <v>27246.73095703125</v>
-      </c>
-      <c r="AG24" s="57">
-        <f t="shared" si="2"/>
-        <v>19461.95068359375</v>
-      </c>
-      <c r="AH24" s="58">
-        <f t="shared" si="12"/>
-        <v>65.545351747557731</v>
-      </c>
-      <c r="AI24" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="51">
-        <f t="shared" si="3"/>
         <v>38923.9013671875</v>
       </c>
       <c r="AK24" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>31139.12109375</v>
       </c>
       <c r="AL24" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>23354.3408203125</v>
       </c>
       <c r="AM24" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>64.195923227443188</v>
       </c>
     </row>
@@ -6668,155 +6692,155 @@
         <v>14</v>
       </c>
       <c r="B25" s="39">
-        <f>B24+B$5*$C$2^($A25)</f>
+        <f t="shared" si="0"/>
         <v>7203.5107872931821</v>
       </c>
       <c r="C25" s="26">
-        <f>C24+C$5*$C$2^($A25)</f>
+        <f t="shared" si="1"/>
         <v>8624.21294475182</v>
       </c>
       <c r="D25" s="26">
-        <f>D24+D$5*$C$2^($A25)</f>
+        <f t="shared" si="2"/>
         <v>7203.5107872931821</v>
       </c>
       <c r="E25" s="40">
-        <f>E24+E$5*$C$2^($A25)</f>
+        <f t="shared" si="3"/>
         <v>5782.808629834547</v>
       </c>
       <c r="F25" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G25" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>23354.3408203125</v>
       </c>
       <c r="H25" s="32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>17515.755615234375</v>
       </c>
       <c r="I25" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>17515.755615234375</v>
       </c>
       <c r="J25" s="45">
+        <f t="shared" si="9"/>
+        <v>135.53043160362239</v>
+      </c>
+      <c r="K25" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="32">
+        <f t="shared" si="8"/>
+        <v>29192.926025390625</v>
+      </c>
+      <c r="M25" s="32">
+        <f t="shared" si="8"/>
+        <v>23354.3408203125</v>
+      </c>
+      <c r="N25" s="33">
+        <f t="shared" si="8"/>
+        <v>17515.755615234375</v>
+      </c>
+      <c r="O25" s="45">
+        <f t="shared" si="10"/>
+        <v>135.53043160362239</v>
+      </c>
+      <c r="P25" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="32">
+        <f t="shared" si="8"/>
+        <v>23354.3408203125</v>
+      </c>
+      <c r="R25" s="32">
+        <f t="shared" si="8"/>
+        <v>29192.926025390625</v>
+      </c>
+      <c r="S25" s="33">
+        <f t="shared" si="8"/>
+        <v>17515.755615234375</v>
+      </c>
+      <c r="T25" s="45">
+        <f t="shared" si="11"/>
+        <v>135.53043160362239</v>
+      </c>
+      <c r="U25" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="32">
+        <f t="shared" si="8"/>
+        <v>17515.755615234375</v>
+      </c>
+      <c r="W25" s="32">
+        <f t="shared" si="8"/>
+        <v>23354.3408203125</v>
+      </c>
+      <c r="X25" s="32">
+        <f t="shared" si="8"/>
+        <v>29192.926025390625</v>
+      </c>
+      <c r="Y25" s="45">
+        <f t="shared" si="12"/>
+        <v>135.53043160362239</v>
+      </c>
+      <c r="Z25" s="52">
+        <f t="shared" si="13"/>
+        <v>305446.48193384241</v>
+      </c>
+      <c r="AA25" s="19">
+        <f t="shared" si="14"/>
+        <v>305446.48193384241</v>
+      </c>
+      <c r="AB25" s="19">
         <f t="shared" si="5"/>
-        <v>135.53043160362239</v>
-      </c>
-      <c r="K25" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="32">
-        <f t="shared" si="4"/>
+        <v>305446.48193384241</v>
+      </c>
+      <c r="AC25" s="19">
+        <f t="shared" si="5"/>
+        <v>305446.48193384241</v>
+      </c>
+      <c r="AD25" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="51">
+        <f t="shared" si="6"/>
+        <v>52547.266845703125</v>
+      </c>
+      <c r="AF25" s="51">
+        <f t="shared" si="6"/>
+        <v>40870.096435546875</v>
+      </c>
+      <c r="AG25" s="57">
+        <f t="shared" si="6"/>
         <v>29192.926025390625</v>
       </c>
-      <c r="M25" s="32">
-        <f t="shared" si="4"/>
-        <v>23354.3408203125</v>
-      </c>
-      <c r="N25" s="33">
-        <f t="shared" si="4"/>
-        <v>17515.755615234375</v>
-      </c>
-      <c r="O25" s="45">
-        <f t="shared" si="6"/>
-        <v>135.53043160362239</v>
-      </c>
-      <c r="P25" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="32">
-        <f t="shared" si="4"/>
-        <v>23354.3408203125</v>
-      </c>
-      <c r="R25" s="32">
-        <f t="shared" si="4"/>
-        <v>29192.926025390625</v>
-      </c>
-      <c r="S25" s="33">
-        <f t="shared" si="4"/>
-        <v>17515.755615234375</v>
-      </c>
-      <c r="T25" s="45">
+      <c r="AH25" s="58">
+        <f t="shared" si="16"/>
+        <v>81.276236166971586</v>
+      </c>
+      <c r="AI25" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="51">
         <f t="shared" si="7"/>
-        <v>135.53043160362239</v>
-      </c>
-      <c r="U25" s="31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V25" s="32">
-        <f t="shared" si="4"/>
-        <v>17515.755615234375</v>
-      </c>
-      <c r="W25" s="32">
-        <f t="shared" si="4"/>
-        <v>23354.3408203125</v>
-      </c>
-      <c r="X25" s="32">
-        <f t="shared" si="4"/>
-        <v>29192.926025390625</v>
-      </c>
-      <c r="Y25" s="45">
-        <f t="shared" si="8"/>
-        <v>135.53043160362239</v>
-      </c>
-      <c r="Z25" s="52">
-        <f t="shared" si="9"/>
-        <v>305446.48193384241</v>
-      </c>
-      <c r="AA25" s="19">
-        <f t="shared" si="10"/>
-        <v>305446.48193384241</v>
-      </c>
-      <c r="AB25" s="19">
-        <f t="shared" si="1"/>
-        <v>305446.48193384241</v>
-      </c>
-      <c r="AC25" s="19">
-        <f t="shared" si="1"/>
-        <v>305446.48193384241</v>
-      </c>
-      <c r="AD25" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE25" s="51">
-        <f t="shared" si="2"/>
-        <v>52547.266845703125</v>
-      </c>
-      <c r="AF25" s="51">
-        <f t="shared" si="2"/>
-        <v>40870.096435546875</v>
-      </c>
-      <c r="AG25" s="57">
-        <f t="shared" si="2"/>
-        <v>29192.926025390625</v>
-      </c>
-      <c r="AH25" s="58">
-        <f t="shared" si="12"/>
-        <v>81.276236166971586</v>
-      </c>
-      <c r="AI25" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ25" s="51">
-        <f t="shared" si="3"/>
         <v>58385.85205078125</v>
       </c>
       <c r="AK25" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>46708.681640625</v>
       </c>
       <c r="AL25" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>35031.51123046875</v>
       </c>
       <c r="AM25" s="58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>77.035107872931817</v>
       </c>
     </row>
@@ -6825,155 +6849,155 @@
         <v>15</v>
       </c>
       <c r="B26" s="41">
-        <f>B25+B$5*$C$2^($A26)</f>
+        <f t="shared" si="0"/>
         <v>8744.2129447518182</v>
       </c>
       <c r="C26" s="42">
-        <f>C25+C$5*$C$2^($A26)</f>
+        <f t="shared" si="1"/>
         <v>10473.055533702183</v>
       </c>
       <c r="D26" s="42">
-        <f>D25+D$5*$C$2^($A26)</f>
+        <f t="shared" si="2"/>
         <v>8744.2129447518182</v>
       </c>
       <c r="E26" s="43">
-        <f>E25+E$5*$C$2^($A26)</f>
+        <f t="shared" si="3"/>
         <v>7015.3703558014558</v>
       </c>
       <c r="F26" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G26" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>35031.51123046875</v>
       </c>
       <c r="H26" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>26273.633422851563</v>
       </c>
       <c r="I26" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>26273.633422851563</v>
       </c>
       <c r="J26" s="46">
+        <f t="shared" si="9"/>
+        <v>192.45321287714378</v>
+      </c>
+      <c r="K26" s="34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="35">
+        <f t="shared" si="8"/>
+        <v>43789.389038085938</v>
+      </c>
+      <c r="M26" s="35">
+        <f t="shared" si="8"/>
+        <v>35031.51123046875</v>
+      </c>
+      <c r="N26" s="36">
+        <f t="shared" si="8"/>
+        <v>26273.633422851563</v>
+      </c>
+      <c r="O26" s="46">
+        <f t="shared" si="10"/>
+        <v>192.45321287714378</v>
+      </c>
+      <c r="P26" s="34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="35">
+        <f t="shared" si="8"/>
+        <v>35031.51123046875</v>
+      </c>
+      <c r="R26" s="35">
+        <f t="shared" si="8"/>
+        <v>43789.389038085938</v>
+      </c>
+      <c r="S26" s="36">
+        <f t="shared" si="8"/>
+        <v>26273.633422851563</v>
+      </c>
+      <c r="T26" s="46">
+        <f t="shared" si="11"/>
+        <v>192.45321287714378</v>
+      </c>
+      <c r="U26" s="34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="35">
+        <f t="shared" si="8"/>
+        <v>26273.633422851563</v>
+      </c>
+      <c r="W26" s="35">
+        <f t="shared" si="8"/>
+        <v>35031.51123046875</v>
+      </c>
+      <c r="X26" s="35">
+        <f t="shared" si="8"/>
+        <v>43789.389038085938</v>
+      </c>
+      <c r="Y26" s="46">
+        <f t="shared" si="12"/>
+        <v>192.45321287714378</v>
+      </c>
+      <c r="Z26" s="53">
+        <f t="shared" si="13"/>
+        <v>500932.23037150153</v>
+      </c>
+      <c r="AA26" s="54">
+        <f t="shared" si="14"/>
+        <v>500932.23037150153</v>
+      </c>
+      <c r="AB26" s="54">
         <f t="shared" si="5"/>
-        <v>192.45321287714378</v>
-      </c>
-      <c r="K26" s="34">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="35">
-        <f t="shared" si="4"/>
+        <v>500932.23037150153</v>
+      </c>
+      <c r="AC26" s="54">
+        <f t="shared" si="5"/>
+        <v>500932.23037150153</v>
+      </c>
+      <c r="AD26" s="51">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="51">
+        <f t="shared" si="6"/>
+        <v>78820.900268554688</v>
+      </c>
+      <c r="AF26" s="51">
+        <f t="shared" si="6"/>
+        <v>61305.144653320313</v>
+      </c>
+      <c r="AG26" s="57">
+        <f t="shared" si="6"/>
         <v>43789.389038085938</v>
       </c>
-      <c r="M26" s="35">
-        <f t="shared" si="4"/>
-        <v>35031.51123046875</v>
-      </c>
-      <c r="N26" s="36">
-        <f t="shared" si="4"/>
-        <v>26273.633422851563</v>
-      </c>
-      <c r="O26" s="46">
-        <f t="shared" si="6"/>
-        <v>192.45321287714378</v>
-      </c>
-      <c r="P26" s="34">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="35">
-        <f t="shared" si="4"/>
-        <v>35031.51123046875</v>
-      </c>
-      <c r="R26" s="35">
-        <f t="shared" si="4"/>
-        <v>43789.389038085938</v>
-      </c>
-      <c r="S26" s="36">
-        <f t="shared" si="4"/>
-        <v>26273.633422851563</v>
-      </c>
-      <c r="T26" s="46">
+      <c r="AH26" s="59">
+        <f t="shared" si="16"/>
+        <v>100.78253284704478</v>
+      </c>
+      <c r="AI26" s="65">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="51">
         <f t="shared" si="7"/>
-        <v>192.45321287714378</v>
-      </c>
-      <c r="U26" s="34">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V26" s="35">
-        <f t="shared" si="4"/>
-        <v>26273.633422851563</v>
-      </c>
-      <c r="W26" s="35">
-        <f t="shared" si="4"/>
-        <v>35031.51123046875</v>
-      </c>
-      <c r="X26" s="35">
-        <f t="shared" si="4"/>
-        <v>43789.389038085938</v>
-      </c>
-      <c r="Y26" s="46">
-        <f t="shared" si="8"/>
-        <v>192.45321287714378</v>
-      </c>
-      <c r="Z26" s="53">
-        <f t="shared" si="9"/>
-        <v>500932.23037150153</v>
-      </c>
-      <c r="AA26" s="54">
-        <f t="shared" si="10"/>
-        <v>500932.23037150153</v>
-      </c>
-      <c r="AB26" s="54">
-        <f t="shared" si="1"/>
-        <v>500932.23037150153</v>
-      </c>
-      <c r="AC26" s="54">
-        <f t="shared" si="1"/>
-        <v>500932.23037150153</v>
-      </c>
-      <c r="AD26" s="51">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE26" s="51">
-        <f t="shared" si="2"/>
-        <v>78820.900268554688</v>
-      </c>
-      <c r="AF26" s="51">
-        <f t="shared" si="2"/>
-        <v>61305.144653320313</v>
-      </c>
-      <c r="AG26" s="57">
-        <f t="shared" si="2"/>
-        <v>43789.389038085938</v>
-      </c>
-      <c r="AH26" s="59">
-        <f t="shared" si="12"/>
-        <v>100.78253284704478</v>
-      </c>
-      <c r="AI26" s="65">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="51">
-        <f t="shared" si="3"/>
         <v>87578.778076171875</v>
       </c>
       <c r="AK26" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>70063.0224609375</v>
       </c>
       <c r="AL26" s="57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>52547.266845703125</v>
       </c>
       <c r="AM26" s="59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>92.442129447518184</v>
       </c>
     </row>
@@ -6984,83 +7008,83 @@
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22">
-        <f t="shared" ref="F27:I27" si="15">SUM(F11:F26)</f>
+        <f t="shared" ref="F27:I27" si="19">SUM(F11:F26)</f>
         <v>0</v>
       </c>
       <c r="G27" s="22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>104879.53369140625</v>
       </c>
       <c r="H27" s="22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>78665.900268554688</v>
       </c>
       <c r="I27" s="22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>78655.900268554688</v>
       </c>
-      <c r="J27" s="92">
+      <c r="J27" s="66">
         <f>SUM(J11:J26)</f>
         <v>649.29419591796238</v>
       </c>
       <c r="K27" s="22">
-        <f t="shared" ref="K27" si="16">SUM(K11:K26)</f>
+        <f t="shared" ref="K27" si="20">SUM(K11:K26)</f>
         <v>0</v>
       </c>
       <c r="L27" s="22">
-        <f t="shared" ref="L27" si="17">SUM(L11:L26)</f>
+        <f t="shared" ref="L27" si="21">SUM(L11:L26)</f>
         <v>131098.16711425781</v>
       </c>
       <c r="M27" s="22">
-        <f t="shared" ref="M27" si="18">SUM(M11:M26)</f>
+        <f t="shared" ref="M27" si="22">SUM(M11:M26)</f>
         <v>104894.53369140625</v>
       </c>
       <c r="N27" s="22">
-        <f t="shared" ref="N27:O27" si="19">SUM(N11:N26)</f>
+        <f t="shared" ref="N27:O27" si="23">SUM(N11:N26)</f>
         <v>78660.900268554688</v>
       </c>
-      <c r="O27" s="92">
-        <f t="shared" si="19"/>
-        <v>649.29419591796238</v>
-      </c>
-      <c r="P27" s="22">
-        <f t="shared" ref="P27" si="20">SUM(P11:P26)</f>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="22">
-        <f t="shared" ref="Q27" si="21">SUM(Q11:Q26)</f>
-        <v>104894.53369140625</v>
-      </c>
-      <c r="R27" s="22">
-        <f t="shared" ref="R27" si="22">SUM(R11:R26)</f>
-        <v>131098.16711425781</v>
-      </c>
-      <c r="S27" s="22">
-        <f t="shared" ref="S27:T27" si="23">SUM(S11:S26)</f>
-        <v>78665.900268554688</v>
-      </c>
-      <c r="T27" s="92">
+      <c r="O27" s="66">
         <f t="shared" si="23"/>
         <v>649.29419591796238</v>
       </c>
+      <c r="P27" s="22">
+        <f t="shared" ref="P27" si="24">SUM(P11:P26)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="22">
+        <f t="shared" ref="Q27" si="25">SUM(Q11:Q26)</f>
+        <v>104894.53369140625</v>
+      </c>
+      <c r="R27" s="22">
+        <f t="shared" ref="R27" si="26">SUM(R11:R26)</f>
+        <v>131098.16711425781</v>
+      </c>
+      <c r="S27" s="22">
+        <f t="shared" ref="S27:T27" si="27">SUM(S11:S26)</f>
+        <v>78665.900268554688</v>
+      </c>
+      <c r="T27" s="66">
+        <f t="shared" si="27"/>
+        <v>649.29419591796238</v>
+      </c>
       <c r="U27" s="22">
-        <f t="shared" ref="U27" si="24">SUM(U11:U26)</f>
+        <f t="shared" ref="U27" si="28">SUM(U11:U26)</f>
         <v>0</v>
       </c>
       <c r="V27" s="22">
-        <f t="shared" ref="V27" si="25">SUM(V11:V26)</f>
+        <f t="shared" ref="V27" si="29">SUM(V11:V26)</f>
         <v>78690.900268554688</v>
       </c>
       <c r="W27" s="22">
-        <f t="shared" ref="W27" si="26">SUM(W11:W26)</f>
+        <f t="shared" ref="W27" si="30">SUM(W11:W26)</f>
         <v>104914.53369140625</v>
       </c>
       <c r="X27" s="22">
-        <f t="shared" ref="X27:Y27" si="27">SUM(X11:X26)</f>
+        <f t="shared" ref="X27:Y27" si="31">SUM(X11:X26)</f>
         <v>131098.16711425781</v>
       </c>
-      <c r="Y27" s="92">
-        <f t="shared" si="27"/>
+      <c r="Y27" s="66">
+        <f t="shared" si="31"/>
         <v>649.29419591796238</v>
       </c>
       <c r="Z27" s="22"/>
@@ -7068,43 +7092,43 @@
       <c r="AB27" s="22"/>
       <c r="AC27" s="22"/>
       <c r="AD27" s="22">
-        <f t="shared" ref="AC27:AD27" si="28">SUM(AD11:AD26)</f>
+        <f t="shared" ref="AD27" si="32">SUM(AD11:AD26)</f>
         <v>0</v>
       </c>
       <c r="AE27" s="22">
-        <f t="shared" ref="AE27" si="29">SUM(AE11:AE26)</f>
+        <f t="shared" ref="AE27" si="33">SUM(AE11:AE26)</f>
         <v>235982.70080566406</v>
       </c>
       <c r="AF27" s="22">
-        <f t="shared" ref="AF27" si="30">SUM(AF11:AF26)</f>
+        <f t="shared" ref="AF27" si="34">SUM(AF11:AF26)</f>
         <v>183570.43395996094</v>
       </c>
       <c r="AG27" s="22">
-        <f t="shared" ref="AG27" si="31">SUM(AG11:AG26)</f>
+        <f t="shared" ref="AG27" si="35">SUM(AG11:AG26)</f>
         <v>131108.16711425781</v>
       </c>
-      <c r="AH27" s="92">
-        <f t="shared" ref="AH27:AI27" si="32">SUM(AH11:AH26)</f>
+      <c r="AH27" s="66">
+        <f t="shared" ref="AH27:AI27" si="36">SUM(AH11:AH26)</f>
         <v>503.04308637639792</v>
       </c>
       <c r="AI27" s="22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AJ27" s="22">
-        <f t="shared" ref="AJ27" si="33">SUM(AJ11:AJ26)</f>
+        <f t="shared" ref="AJ27" si="37">SUM(AJ11:AJ26)</f>
         <v>262206.33422851563</v>
       </c>
       <c r="AK27" s="22">
-        <f t="shared" ref="AK27" si="34">SUM(AK11:AK26)</f>
+        <f t="shared" ref="AK27" si="38">SUM(AK11:AK26)</f>
         <v>209799.0673828125</v>
       </c>
       <c r="AL27" s="22">
-        <f t="shared" ref="AL27" si="35">SUM(AL11:AL26)</f>
+        <f t="shared" ref="AL27" si="39">SUM(AL11:AL26)</f>
         <v>157331.80053710938</v>
       </c>
-      <c r="AM27" s="92">
-        <f t="shared" ref="AM27" si="36">SUM(AM11:AM26)</f>
+      <c r="AM27" s="66">
+        <f t="shared" ref="AM27" si="40">SUM(AM11:AM26)</f>
         <v>522.65277668510919</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add troop action to frontend
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitd\minute_empire\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4940251E-05DF-49DA-B52D-46130B10A60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1D84C0-F3F9-41C3-A935-30C2B3DC79DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
   </bookViews>
@@ -1064,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1290,12 +1290,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1332,8 +1335,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1671,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160B8A5D-57A4-491A-8F64-525E78E348B7}">
   <dimension ref="A1:AU69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="AJ24" sqref="AJ24"/>
+    <sheetView tabSelected="1" topLeftCell="J22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2008,7 @@
       <c r="N30" s="19"/>
       <c r="O30" s="19"/>
       <c r="P30" s="19"/>
-      <c r="Q30" s="20"/>
+      <c r="Q30" s="106"/>
       <c r="R30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -2013,7 +2016,7 @@
       <c r="V30" s="19"/>
       <c r="W30" s="19"/>
       <c r="X30" s="19"/>
-      <c r="Y30" s="20"/>
+      <c r="Y30" s="106"/>
       <c r="Z30" s="19"/>
       <c r="AA30" s="19"/>
       <c r="AB30" s="19"/>
@@ -2047,9 +2050,9 @@
       </c>
       <c r="N31" s="19"/>
       <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
+      <c r="P31" s="20"/>
       <c r="Q31" s="20"/>
-      <c r="R31" s="19"/>
+      <c r="R31" s="20"/>
       <c r="S31" s="19"/>
       <c r="T31" s="19"/>
       <c r="U31" s="19"/>
@@ -2092,17 +2095,17 @@
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="N32" s="19"/>
-      <c r="O32" s="20"/>
+      <c r="O32" s="106"/>
       <c r="P32" s="20"/>
       <c r="Q32" s="21" t="s">
         <v>35</v>
       </c>
       <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
+      <c r="S32" s="106"/>
       <c r="T32" s="19"/>
       <c r="U32" s="19"/>
       <c r="V32" s="19"/>
-      <c r="W32" s="20"/>
+      <c r="W32" s="106"/>
       <c r="X32" s="20" t="s">
         <v>35</v>
       </c>
@@ -2110,7 +2113,7 @@
       <c r="Z32" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AA32" s="20"/>
+      <c r="AA32" s="106"/>
       <c r="AB32" s="19"/>
       <c r="AC32" s="19"/>
       <c r="AD32" s="19"/>
@@ -2142,9 +2145,9 @@
       </c>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
+      <c r="P33" s="20"/>
       <c r="Q33" s="20"/>
-      <c r="R33" s="19"/>
+      <c r="R33" s="20"/>
       <c r="S33" s="19"/>
       <c r="T33" s="19"/>
       <c r="U33" s="19"/>
@@ -2192,7 +2195,7 @@
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
-      <c r="Q34" s="20"/>
+      <c r="Q34" s="106"/>
       <c r="R34" s="19"/>
       <c r="S34" s="19"/>
       <c r="T34" s="19"/>
@@ -2200,7 +2203,7 @@
       <c r="V34" s="19"/>
       <c r="W34" s="19"/>
       <c r="X34" s="19"/>
-      <c r="Y34" s="20"/>
+      <c r="Y34" s="106"/>
       <c r="Z34" s="19"/>
       <c r="AA34" s="19"/>
       <c r="AB34" s="19"/>
@@ -4088,12 +4091,12 @@
       <c r="W3" s="92"/>
       <c r="X3" s="92"/>
       <c r="Y3" s="92"/>
-      <c r="Z3" s="96" t="s">
+      <c r="Z3" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="96"/>
-      <c r="AB3" s="96"/>
-      <c r="AC3" s="96"/>
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="97"/>
       <c r="AD3" s="19"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -4131,14 +4134,14 @@
       <c r="W4" s="92"/>
       <c r="X4" s="92"/>
       <c r="Y4" s="84"/>
-      <c r="Z4" s="96" t="s">
+      <c r="Z4" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="96" t="s">
+      <c r="AA4" s="97"/>
+      <c r="AB4" s="97" t="s">
         <v>77</v>
       </c>
-      <c r="AC4" s="96"/>
+      <c r="AC4" s="97"/>
       <c r="AD4" s="92" t="s">
         <v>82</v>
       </c>
@@ -4324,28 +4327,28 @@
       <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="102" t="s">
+      <c r="F8" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="103"/>
-      <c r="X8" s="103"/>
-      <c r="Y8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="104"/>
+      <c r="P8" s="104"/>
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="104"/>
+      <c r="T8" s="104"/>
+      <c r="U8" s="104"/>
+      <c r="V8" s="104"/>
+      <c r="W8" s="104"/>
+      <c r="X8" s="104"/>
+      <c r="Y8" s="105"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
@@ -4354,55 +4357,55 @@
       </c>
       <c r="C9" s="90"/>
       <c r="D9" s="90"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="97" t="s">
+      <c r="E9" s="91"/>
+      <c r="F9" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="97" t="s">
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="99"/>
-      <c r="P9" s="97" t="s">
+      <c r="L9" s="99"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="99"/>
+      <c r="O9" s="100"/>
+      <c r="P9" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="98"/>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="99"/>
-      <c r="U9" s="100" t="s">
+      <c r="Q9" s="99"/>
+      <c r="R9" s="99"/>
+      <c r="S9" s="99"/>
+      <c r="T9" s="100"/>
+      <c r="U9" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="101"/>
-      <c r="W9" s="101"/>
-      <c r="X9" s="101"/>
-      <c r="Y9" s="101"/>
-      <c r="Z9" s="93" t="s">
+      <c r="V9" s="102"/>
+      <c r="W9" s="102"/>
+      <c r="X9" s="102"/>
+      <c r="Y9" s="102"/>
+      <c r="Z9" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="94"/>
-      <c r="AB9" s="94"/>
-      <c r="AC9" s="95"/>
+      <c r="AA9" s="95"/>
+      <c r="AB9" s="95"/>
+      <c r="AC9" s="96"/>
       <c r="AD9" s="89" t="s">
         <v>81</v>
       </c>
       <c r="AE9" s="90"/>
       <c r="AF9" s="90"/>
       <c r="AG9" s="90"/>
-      <c r="AH9" s="91"/>
+      <c r="AH9" s="93"/>
       <c r="AI9" s="89" t="s">
         <v>80</v>
       </c>
       <c r="AJ9" s="90"/>
       <c r="AK9" s="90"/>
       <c r="AL9" s="90"/>
-      <c r="AM9" s="91"/>
+      <c r="AM9" s="93"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
@@ -7188,11 +7191,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="P4:S4"/>
     <mergeCell ref="AI9:AM9"/>
     <mergeCell ref="AD9:AH9"/>
     <mergeCell ref="AD4:AH4"/>
@@ -7208,6 +7206,11 @@
     <mergeCell ref="P9:T9"/>
     <mergeCell ref="U9:Y9"/>
     <mergeCell ref="F8:Y8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="P4:S4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
improve troops action display
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitd\minute_empire\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1D84C0-F3F9-41C3-A935-30C2B3DC79DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BA587-35B6-4876-B660-704B5CF9BB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
   </bookViews>
   <sheets>
     <sheet name="brainstorming" sheetId="1" r:id="rId1"/>
-    <sheet name="Feedbacks" sheetId="2" r:id="rId2"/>
-    <sheet name="Dinâmica de jogo" sheetId="3" r:id="rId3"/>
-    <sheet name="Timeline" sheetId="4" r:id="rId4"/>
-    <sheet name="Tempo recursos" sheetId="5" r:id="rId5"/>
+    <sheet name="Troops" sheetId="6" r:id="rId2"/>
+    <sheet name="Feedbacks" sheetId="2" r:id="rId3"/>
+    <sheet name="Dinâmica de jogo" sheetId="3" r:id="rId4"/>
+    <sheet name="Timeline" sheetId="4" r:id="rId5"/>
+    <sheet name="Tempo recursos" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="95">
   <si>
     <t>Collections</t>
   </si>
@@ -313,6 +314,18 @@
   </si>
   <si>
     <t>Custos das construções vai variar de acordo com o nível que eu quero que o pessoal construa ela</t>
+  </si>
+  <si>
+    <t>Longbowman</t>
+  </si>
+  <si>
+    <t>Crossbowman</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1290,53 +1303,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1353,6 +1370,133 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C85A4208-873A-1745-EC9C-363696A95984}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10306050" y="2952750"/>
+          <a:ext cx="790575" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Retângulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F0F64A-1C33-487B-9491-C5BA630789FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10115550" y="2781300"/>
+          <a:ext cx="1181100" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1674,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160B8A5D-57A4-491A-8F64-525E78E348B7}">
   <dimension ref="A1:AU69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J22" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView topLeftCell="D24" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27:AR35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,108 +2082,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="O28" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="80"/>
-      <c r="R28" s="80"/>
-      <c r="S28" s="80"/>
-      <c r="W28" s="80" t="s">
-        <v>36</v>
-      </c>
-      <c r="X28" s="80"/>
-      <c r="Y28" s="80"/>
-      <c r="Z28" s="80"/>
-      <c r="AA28" s="80"/>
-      <c r="AD28" s="80" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE28" s="80"/>
-      <c r="AF28" s="80"/>
-      <c r="AG28" s="80"/>
-      <c r="AH28" s="80"/>
-      <c r="AL28" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM28" s="80"/>
-      <c r="AN28" s="80"/>
-      <c r="AO28" s="80"/>
-      <c r="AP28" s="80"/>
-    </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
-      <c r="W29" s="19"/>
-      <c r="X29" s="19"/>
-      <c r="Y29" s="19"/>
-      <c r="Z29" s="19"/>
-      <c r="AA29" s="19"/>
-      <c r="AB29" s="19"/>
-      <c r="AC29" s="19"/>
-      <c r="AD29" s="19"/>
-      <c r="AE29" s="19"/>
-      <c r="AF29" s="19"/>
-      <c r="AG29" s="19"/>
-      <c r="AH29" s="19"/>
-      <c r="AI29" s="19"/>
-      <c r="AJ29" s="19"/>
-      <c r="AK29" s="19"/>
-      <c r="AL29" s="19"/>
-      <c r="AM29" s="19"/>
-      <c r="AN29" s="19"/>
-      <c r="AO29" s="19"/>
-      <c r="AP29" s="19"/>
-      <c r="AQ29" s="19"/>
-      <c r="AR29" s="19"/>
       <c r="AS29" s="19"/>
       <c r="AT29" s="19"/>
       <c r="AU29" s="19"/>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="106"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="19"/>
-      <c r="X30" s="19"/>
-      <c r="Y30" s="106"/>
-      <c r="Z30" s="19"/>
-      <c r="AA30" s="19"/>
-      <c r="AB30" s="19"/>
-      <c r="AC30" s="19"/>
-      <c r="AD30" s="19"/>
-      <c r="AE30" s="20"/>
-      <c r="AF30" s="19"/>
-      <c r="AG30" s="20"/>
-      <c r="AH30" s="19"/>
-      <c r="AI30" s="19"/>
-      <c r="AJ30" s="19"/>
-      <c r="AK30" s="19"/>
-      <c r="AL30" s="19"/>
-      <c r="AM30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN30" s="19"/>
-      <c r="AO30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP30" s="19"/>
-      <c r="AQ30" s="19"/>
-      <c r="AR30" s="19"/>
       <c r="AS30" s="19"/>
       <c r="AT30" s="19"/>
       <c r="AU30" s="19"/>
@@ -2048,93 +2096,11 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="19"/>
-      <c r="X31" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z31" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA31" s="19"/>
-      <c r="AB31" s="19"/>
-      <c r="AC31" s="19"/>
-      <c r="AD31" s="20"/>
-      <c r="AE31" s="19"/>
-      <c r="AF31" s="19"/>
-      <c r="AG31" s="19"/>
-      <c r="AH31" s="20"/>
-      <c r="AI31" s="19"/>
-      <c r="AJ31" s="19"/>
-      <c r="AK31" s="19"/>
-      <c r="AL31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM31" s="20"/>
-      <c r="AN31" s="20"/>
-      <c r="AO31" s="20"/>
-      <c r="AP31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ31" s="19"/>
-      <c r="AR31" s="19"/>
       <c r="AS31" s="19"/>
       <c r="AT31" s="19"/>
       <c r="AU31" s="19"/>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="N32" s="19"/>
-      <c r="O32" s="106"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="R32" s="20"/>
-      <c r="S32" s="106"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="106"/>
-      <c r="X32" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y32" s="21"/>
-      <c r="Z32" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA32" s="106"/>
-      <c r="AB32" s="19"/>
-      <c r="AC32" s="19"/>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="19"/>
-      <c r="AF32" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG32" s="19"/>
-      <c r="AH32" s="19"/>
-      <c r="AI32" s="19"/>
-      <c r="AJ32" s="19"/>
-      <c r="AK32" s="19"/>
-      <c r="AL32" s="19"/>
-      <c r="AM32" s="20"/>
-      <c r="AN32" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO32" s="20"/>
-      <c r="AP32" s="19"/>
-      <c r="AQ32" s="19"/>
-      <c r="AR32" s="19"/>
       <c r="AS32" s="19"/>
       <c r="AT32" s="19"/>
       <c r="AU32" s="19"/>
@@ -2143,47 +2109,6 @@
       <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
-      <c r="X33" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y33" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z33" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA33" s="19"/>
-      <c r="AB33" s="19"/>
-      <c r="AC33" s="19"/>
-      <c r="AD33" s="20"/>
-      <c r="AE33" s="19"/>
-      <c r="AF33" s="19"/>
-      <c r="AG33" s="19"/>
-      <c r="AH33" s="20"/>
-      <c r="AI33" s="19"/>
-      <c r="AJ33" s="19"/>
-      <c r="AK33" s="19"/>
-      <c r="AL33" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM33" s="20"/>
-      <c r="AN33" s="20"/>
-      <c r="AO33" s="20"/>
-      <c r="AP33" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ33" s="19"/>
-      <c r="AR33" s="19"/>
       <c r="AS33" s="19"/>
       <c r="AT33" s="19"/>
       <c r="AU33" s="19"/>
@@ -2192,41 +2117,6 @@
       <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="106"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="19"/>
-      <c r="Y34" s="106"/>
-      <c r="Z34" s="19"/>
-      <c r="AA34" s="19"/>
-      <c r="AB34" s="19"/>
-      <c r="AC34" s="19"/>
-      <c r="AD34" s="19"/>
-      <c r="AE34" s="20"/>
-      <c r="AF34" s="19"/>
-      <c r="AG34" s="20"/>
-      <c r="AH34" s="19"/>
-      <c r="AI34" s="19"/>
-      <c r="AJ34" s="19"/>
-      <c r="AK34" s="19"/>
-      <c r="AL34" s="19"/>
-      <c r="AM34" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN34" s="19"/>
-      <c r="AO34" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP34" s="19"/>
-      <c r="AQ34" s="19"/>
-      <c r="AR34" s="19"/>
       <c r="AS34" s="19"/>
       <c r="AT34" s="19"/>
       <c r="AU34" s="19"/>
@@ -2235,37 +2125,6 @@
       <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="19"/>
-      <c r="X35" s="19"/>
-      <c r="Y35" s="19"/>
-      <c r="Z35" s="19"/>
-      <c r="AA35" s="19"/>
-      <c r="AB35" s="19"/>
-      <c r="AC35" s="19"/>
-      <c r="AD35" s="19"/>
-      <c r="AE35" s="19"/>
-      <c r="AF35" s="19"/>
-      <c r="AG35" s="19"/>
-      <c r="AH35" s="19"/>
-      <c r="AI35" s="19"/>
-      <c r="AJ35" s="19"/>
-      <c r="AK35" s="19"/>
-      <c r="AL35" s="19"/>
-      <c r="AM35" s="19"/>
-      <c r="AN35" s="19"/>
-      <c r="AO35" s="19"/>
-      <c r="AP35" s="19"/>
-      <c r="AQ35" s="19"/>
-      <c r="AR35" s="19"/>
       <c r="AS35" s="19"/>
       <c r="AT35" s="19"/>
       <c r="AU35" s="19"/>
@@ -3709,18 +3568,645 @@
       <c r="AT69" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="O28:S28"/>
-    <mergeCell ref="W28:AA28"/>
-    <mergeCell ref="AD28:AH28"/>
-    <mergeCell ref="AL28:AP28"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC303E8-E0FB-43A9-8BA9-B72A37BC53D0}">
+  <dimension ref="A2:BG30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AR17" sqref="AR17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="74" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B2" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="J2" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="W2" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
+      <c r="Z2" s="80"/>
+      <c r="AA2" s="80"/>
+      <c r="AM2" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN2" s="80"/>
+      <c r="AO2" s="80"/>
+      <c r="AP2" s="80"/>
+      <c r="AQ2" s="80"/>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="19"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO4" s="19"/>
+      <c r="AP4" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ4" s="19"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="20"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AM5" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="107" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AM6" s="19"/>
+      <c r="AN6" s="20"/>
+      <c r="AO6" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="19"/>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="20"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AM7" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
+      <c r="AQ7" s="107" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AM8" s="19"/>
+      <c r="AN8" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO8" s="19"/>
+      <c r="AP8" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ8" s="19"/>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="19"/>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="19"/>
+      <c r="AE9" s="19"/>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="J12" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="W12" s="80" t="s">
+        <v>94</v>
+      </c>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="80"/>
+      <c r="AA12" s="80"/>
+      <c r="AZ12" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA12" s="80"/>
+      <c r="BB12" s="80"/>
+      <c r="BC12" s="80"/>
+      <c r="BD12" s="80"/>
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14" s="106"/>
+      <c r="Y14" s="106"/>
+      <c r="AA14" s="106"/>
+    </row>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" t="s">
+        <v>35</v>
+      </c>
+      <c r="V15" s="106"/>
+      <c r="AB15" s="106"/>
+      <c r="AY15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF15" s="22"/>
+      <c r="BG15" s="22"/>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" t="s">
+        <v>35</v>
+      </c>
+      <c r="U16" s="106"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="19"/>
+      <c r="AC16" s="106"/>
+      <c r="AY16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF16" s="22"/>
+      <c r="BG16" s="22"/>
+    </row>
+    <row r="17" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="K17" s="19"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="19"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="20"/>
+      <c r="AY17" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ17" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA17" s="22"/>
+      <c r="BB17" s="108"/>
+      <c r="BC17" s="22"/>
+      <c r="BD17" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE17" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF17" s="22"/>
+      <c r="BG17" s="22"/>
+    </row>
+    <row r="18" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="20"/>
+      <c r="U18" s="106"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AC18" s="106"/>
+      <c r="AY18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA18" s="108"/>
+      <c r="BB18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC18" s="108"/>
+      <c r="BD18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF18" s="22"/>
+      <c r="BG18" s="22"/>
+    </row>
+    <row r="19" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="K19" s="19"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="19"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="20"/>
+      <c r="AY19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA19" s="22"/>
+      <c r="BB19" s="108"/>
+      <c r="BC19" s="22"/>
+      <c r="BD19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF19" s="22"/>
+      <c r="BG19" s="22"/>
+    </row>
+    <row r="20" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="U20" s="106"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="19"/>
+      <c r="AC20" s="106"/>
+      <c r="AY20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF20" s="22"/>
+      <c r="BG20" s="22"/>
+    </row>
+    <row r="21" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>35</v>
+      </c>
+      <c r="V21" s="106"/>
+      <c r="AB21" s="106"/>
+      <c r="AY21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BD21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF21" s="22"/>
+      <c r="BG21" s="22"/>
+    </row>
+    <row r="22" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>35</v>
+      </c>
+      <c r="W22" s="106"/>
+      <c r="Y22" s="106"/>
+      <c r="AA22" s="106"/>
+      <c r="AY22" s="22"/>
+      <c r="AZ22" s="22"/>
+      <c r="BA22" s="22"/>
+      <c r="BB22" s="22"/>
+      <c r="BC22" s="22"/>
+      <c r="BD22" s="22"/>
+      <c r="BE22" s="22"/>
+      <c r="BF22" s="22"/>
+      <c r="BG22" s="22"/>
+    </row>
+    <row r="26" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="J26" s="80" t="s">
+        <v>92</v>
+      </c>
+      <c r="K26" s="80"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+    </row>
+    <row r="28" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="K28" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" s="20"/>
+      <c r="M28" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="K29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M29" s="20"/>
+    </row>
+    <row r="30" spans="8:59" x14ac:dyDescent="0.25">
+      <c r="K30" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" s="20"/>
+      <c r="M30" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="AZ12:BD12"/>
+    <mergeCell ref="W12:AA12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="AM2:AQ2"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="J26:N26"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641E6139-2B81-4C9C-9758-E87C71064412}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -3745,7 +4231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550AAB3F-C06C-4BC4-BC52-26C567DF5A60}">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -3864,7 +4350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA015092-742B-4B09-B582-52072BAD5DCA}">
   <dimension ref="G1:L9"/>
   <sheetViews>
@@ -3964,7 +4450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F995D2-727F-4F0D-94D8-60C72D5EAEAA}">
   <dimension ref="A1:AM31"/>
   <sheetViews>
@@ -4091,12 +4577,12 @@
       <c r="W3" s="92"/>
       <c r="X3" s="92"/>
       <c r="Y3" s="92"/>
-      <c r="Z3" s="97" t="s">
+      <c r="Z3" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
+      <c r="AA3" s="96"/>
+      <c r="AB3" s="96"/>
+      <c r="AC3" s="96"/>
       <c r="AD3" s="19"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -4134,14 +4620,14 @@
       <c r="W4" s="92"/>
       <c r="X4" s="92"/>
       <c r="Y4" s="84"/>
-      <c r="Z4" s="97" t="s">
+      <c r="Z4" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97" t="s">
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="AC4" s="97"/>
+      <c r="AC4" s="96"/>
       <c r="AD4" s="92" t="s">
         <v>82</v>
       </c>
@@ -4327,28 +4813,28 @@
       <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="103" t="s">
+      <c r="F8" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="104"/>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="104"/>
-      <c r="O8" s="104"/>
-      <c r="P8" s="104"/>
-      <c r="Q8" s="104"/>
-      <c r="R8" s="104"/>
-      <c r="S8" s="104"/>
-      <c r="T8" s="104"/>
-      <c r="U8" s="104"/>
-      <c r="V8" s="104"/>
-      <c r="W8" s="104"/>
-      <c r="X8" s="104"/>
-      <c r="Y8" s="105"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="103"/>
+      <c r="X8" s="103"/>
+      <c r="Y8" s="104"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
@@ -4357,55 +4843,55 @@
       </c>
       <c r="C9" s="90"/>
       <c r="D9" s="90"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="98" t="s">
+      <c r="E9" s="105"/>
+      <c r="F9" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="98" t="s">
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="99"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="99"/>
-      <c r="O9" s="100"/>
-      <c r="P9" s="98" t="s">
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="99"/>
+      <c r="P9" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="99"/>
-      <c r="R9" s="99"/>
-      <c r="S9" s="99"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="101" t="s">
+      <c r="Q9" s="98"/>
+      <c r="R9" s="98"/>
+      <c r="S9" s="98"/>
+      <c r="T9" s="99"/>
+      <c r="U9" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="102"/>
-      <c r="W9" s="102"/>
-      <c r="X9" s="102"/>
-      <c r="Y9" s="102"/>
-      <c r="Z9" s="94" t="s">
+      <c r="V9" s="101"/>
+      <c r="W9" s="101"/>
+      <c r="X9" s="101"/>
+      <c r="Y9" s="101"/>
+      <c r="Z9" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="95"/>
-      <c r="AB9" s="95"/>
-      <c r="AC9" s="96"/>
+      <c r="AA9" s="94"/>
+      <c r="AB9" s="94"/>
+      <c r="AC9" s="95"/>
       <c r="AD9" s="89" t="s">
         <v>81</v>
       </c>
       <c r="AE9" s="90"/>
       <c r="AF9" s="90"/>
       <c r="AG9" s="90"/>
-      <c r="AH9" s="93"/>
+      <c r="AH9" s="91"/>
       <c r="AI9" s="89" t="s">
         <v>80</v>
       </c>
       <c r="AJ9" s="90"/>
       <c r="AK9" s="90"/>
       <c r="AL9" s="90"/>
-      <c r="AM9" s="93"/>
+      <c r="AM9" s="91"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
@@ -7191,6 +7677,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="P4:S4"/>
     <mergeCell ref="AI9:AM9"/>
     <mergeCell ref="AD9:AH9"/>
     <mergeCell ref="AD4:AH4"/>
@@ -7206,11 +7697,6 @@
     <mergeCell ref="P9:T9"/>
     <mergeCell ref="U9:Y9"/>
     <mergeCell ref="F8:Y8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="P4:S4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
add troop train display
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitd\minute_empire\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BA587-35B6-4876-B660-704B5CF9BB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3413D8F-6CF6-4D5B-8874-66FDA6BBA3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
   </bookViews>
   <sheets>
     <sheet name="brainstorming" sheetId="1" r:id="rId1"/>
     <sheet name="Troops" sheetId="6" r:id="rId2"/>
     <sheet name="Feedbacks" sheetId="2" r:id="rId3"/>
-    <sheet name="Dinâmica de jogo" sheetId="3" r:id="rId4"/>
-    <sheet name="Timeline" sheetId="4" r:id="rId5"/>
-    <sheet name="Tempo recursos" sheetId="5" r:id="rId6"/>
+    <sheet name="Troops simulator" sheetId="7" r:id="rId4"/>
+    <sheet name="Dinâmica de jogo" sheetId="3" r:id="rId5"/>
+    <sheet name="Timeline" sheetId="4" r:id="rId6"/>
+    <sheet name="Tempo recursos" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="114">
   <si>
     <t>Collections</t>
   </si>
@@ -326,6 +327,63 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>Light cavalary</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Attacker</t>
+  </si>
+  <si>
+    <t>Defender</t>
+  </si>
+  <si>
+    <t>Total attack</t>
+  </si>
+  <si>
+    <t>winner_snowball_parameter</t>
+  </si>
+  <si>
+    <t>Attacker penalty</t>
+  </si>
+  <si>
+    <t>Loss percentage</t>
+  </si>
+  <si>
+    <t>Attack snowball ratio</t>
+  </si>
+  <si>
+    <t>Final troop quantity</t>
+  </si>
+  <si>
+    <t>No survivor threshold</t>
+  </si>
+  <si>
+    <t>Troop attack</t>
+  </si>
+  <si>
+    <t>Troop Defence</t>
+  </si>
+  <si>
+    <t>Has survivors?</t>
+  </si>
+  <si>
+    <t>Calculated final troop quantity</t>
+  </si>
+  <si>
+    <t>Case 1 - Militia vs Militia (attack + defence)</t>
+  </si>
+  <si>
+    <t>All lived?</t>
+  </si>
+  <si>
+    <t>Total Defense</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1270,6 +1328,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1303,12 +1365,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1345,14 +1410,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3577,8 +3647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC303E8-E0FB-43A9-8BA9-B72A37BC53D0}">
   <dimension ref="A2:BG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR17" sqref="AR17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3587,34 +3657,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="J2" s="80" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="J2" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="W2" s="80" t="s">
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="W2" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="80"/>
-      <c r="Z2" s="80"/>
-      <c r="AA2" s="80"/>
-      <c r="AM2" s="80" t="s">
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
+      <c r="AM2" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="AN2" s="80"/>
-      <c r="AO2" s="80"/>
-      <c r="AP2" s="80"/>
-      <c r="AQ2" s="80"/>
+      <c r="AN2" s="82"/>
+      <c r="AO2" s="82"/>
+      <c r="AP2" s="82"/>
+      <c r="AQ2" s="82"/>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
@@ -3673,11 +3743,11 @@
       <c r="AD4" s="19"/>
       <c r="AE4" s="19"/>
       <c r="AM4" s="19"/>
-      <c r="AN4" s="107" t="s">
+      <c r="AN4" s="19" t="s">
         <v>35</v>
       </c>
       <c r="AO4" s="19"/>
-      <c r="AP4" s="107" t="s">
+      <c r="AP4" s="19" t="s">
         <v>35</v>
       </c>
       <c r="AQ4" s="19"/>
@@ -3713,13 +3783,13 @@
       <c r="AA5" s="20"/>
       <c r="AD5" s="19"/>
       <c r="AE5" s="19"/>
-      <c r="AM5" s="107" t="s">
+      <c r="AM5" s="19" t="s">
         <v>35</v>
       </c>
       <c r="AN5" s="20"/>
       <c r="AO5" s="20"/>
       <c r="AP5" s="20"/>
-      <c r="AQ5" s="107" t="s">
+      <c r="AQ5" s="19" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3795,13 +3865,13 @@
       <c r="AA7" s="20"/>
       <c r="AD7" s="19"/>
       <c r="AE7" s="19"/>
-      <c r="AM7" s="107" t="s">
+      <c r="AM7" s="19" t="s">
         <v>35</v>
       </c>
       <c r="AN7" s="20"/>
       <c r="AO7" s="20"/>
       <c r="AP7" s="20"/>
-      <c r="AQ7" s="107" t="s">
+      <c r="AQ7" s="19" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3831,11 +3901,11 @@
       <c r="AD8" s="19"/>
       <c r="AE8" s="19"/>
       <c r="AM8" s="19"/>
-      <c r="AN8" s="107" t="s">
+      <c r="AN8" s="19" t="s">
         <v>35</v>
       </c>
       <c r="AO8" s="19"/>
-      <c r="AP8" s="107" t="s">
+      <c r="AP8" s="19" t="s">
         <v>35</v>
       </c>
       <c r="AQ8" s="19"/>
@@ -3874,27 +3944,27 @@
       <c r="AE9" s="19"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="J12" s="80" t="s">
+      <c r="J12" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="W12" s="80" t="s">
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="W12" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="X12" s="80"/>
-      <c r="Y12" s="80"/>
-      <c r="Z12" s="80"/>
-      <c r="AA12" s="80"/>
-      <c r="AZ12" s="80" t="s">
+      <c r="X12" s="82"/>
+      <c r="Y12" s="82"/>
+      <c r="Z12" s="82"/>
+      <c r="AA12" s="82"/>
+      <c r="AZ12" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="BA12" s="80"/>
-      <c r="BB12" s="80"/>
-      <c r="BC12" s="80"/>
-      <c r="BD12" s="80"/>
+      <c r="BA12" s="82"/>
+      <c r="BB12" s="82"/>
+      <c r="BC12" s="82"/>
+      <c r="BD12" s="82"/>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
@@ -3903,9 +3973,9 @@
       <c r="P14" t="s">
         <v>35</v>
       </c>
-      <c r="W14" s="106"/>
-      <c r="Y14" s="106"/>
-      <c r="AA14" s="106"/>
+      <c r="W14" s="80"/>
+      <c r="Y14" s="80"/>
+      <c r="AA14" s="80"/>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
@@ -3914,8 +3984,8 @@
       <c r="O15" t="s">
         <v>35</v>
       </c>
-      <c r="V15" s="106"/>
-      <c r="AB15" s="106"/>
+      <c r="V15" s="80"/>
+      <c r="AB15" s="80"/>
       <c r="AY15" s="22" t="s">
         <v>35</v>
       </c>
@@ -3947,13 +4017,13 @@
       <c r="N16" t="s">
         <v>35</v>
       </c>
-      <c r="U16" s="106"/>
+      <c r="U16" s="80"/>
       <c r="W16" s="19"/>
       <c r="X16" s="20"/>
       <c r="Y16" s="19"/>
       <c r="Z16" s="20"/>
       <c r="AA16" s="19"/>
-      <c r="AC16" s="106"/>
+      <c r="AC16" s="80"/>
       <c r="AY16" s="22" t="s">
         <v>35</v>
       </c>
@@ -3994,7 +4064,7 @@
         <v>35</v>
       </c>
       <c r="BA17" s="22"/>
-      <c r="BB17" s="108"/>
+      <c r="BB17" s="81"/>
       <c r="BC17" s="22"/>
       <c r="BD17" s="22" t="s">
         <v>35</v>
@@ -4009,7 +4079,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="21"/>
       <c r="M18" s="20"/>
-      <c r="U18" s="106"/>
+      <c r="U18" s="80"/>
       <c r="W18" s="19"/>
       <c r="X18" s="19"/>
       <c r="Y18" s="21" t="s">
@@ -4017,18 +4087,18 @@
       </c>
       <c r="Z18" s="19"/>
       <c r="AA18" s="19"/>
-      <c r="AC18" s="106"/>
+      <c r="AC18" s="80"/>
       <c r="AY18" s="22" t="s">
         <v>35</v>
       </c>
       <c r="AZ18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="BA18" s="108"/>
+      <c r="BA18" s="81"/>
       <c r="BB18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="BC18" s="108"/>
+      <c r="BC18" s="81"/>
       <c r="BD18" s="22" t="s">
         <v>35</v>
       </c>
@@ -4054,7 +4124,7 @@
         <v>35</v>
       </c>
       <c r="BA19" s="22"/>
-      <c r="BB19" s="108"/>
+      <c r="BB19" s="81"/>
       <c r="BC19" s="22"/>
       <c r="BD19" s="22" t="s">
         <v>35</v>
@@ -4072,13 +4142,13 @@
       <c r="N20" t="s">
         <v>35</v>
       </c>
-      <c r="U20" s="106"/>
+      <c r="U20" s="80"/>
       <c r="W20" s="19"/>
       <c r="X20" s="20"/>
       <c r="Y20" s="19"/>
       <c r="Z20" s="20"/>
       <c r="AA20" s="19"/>
-      <c r="AC20" s="106"/>
+      <c r="AC20" s="80"/>
       <c r="AY20" s="22" t="s">
         <v>35</v>
       </c>
@@ -4110,8 +4180,8 @@
       <c r="O21" t="s">
         <v>35</v>
       </c>
-      <c r="V21" s="106"/>
-      <c r="AB21" s="106"/>
+      <c r="V21" s="80"/>
+      <c r="AB21" s="80"/>
       <c r="AY21" s="22" t="s">
         <v>35</v>
       </c>
@@ -4143,9 +4213,9 @@
       <c r="P22" t="s">
         <v>35</v>
       </c>
-      <c r="W22" s="106"/>
-      <c r="Y22" s="106"/>
-      <c r="AA22" s="106"/>
+      <c r="W22" s="80"/>
+      <c r="Y22" s="80"/>
+      <c r="AA22" s="80"/>
       <c r="AY22" s="22"/>
       <c r="AZ22" s="22"/>
       <c r="BA22" s="22"/>
@@ -4157,13 +4227,13 @@
       <c r="BG22" s="22"/>
     </row>
     <row r="26" spans="8:59" x14ac:dyDescent="0.25">
-      <c r="J26" s="80" t="s">
+      <c r="J26" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-      <c r="M26" s="80"/>
-      <c r="N26" s="80"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
+      <c r="N26" s="82"/>
     </row>
     <row r="28" spans="8:59" x14ac:dyDescent="0.25">
       <c r="K28" s="19" t="s">
@@ -4192,6 +4262,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="J26:N26"/>
     <mergeCell ref="AZ12:BD12"/>
     <mergeCell ref="W12:AA12"/>
     <mergeCell ref="B2:F2"/>
@@ -4199,7 +4270,6 @@
     <mergeCell ref="W2:AA2"/>
     <mergeCell ref="AM2:AQ2"/>
     <mergeCell ref="J12:N12"/>
-    <mergeCell ref="J26:N26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -4232,6 +4302,417 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139C9724-4F9F-4074-A497-A1553C1D940C}">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="K1" s="109" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="110"/>
+      <c r="S1" s="110"/>
+      <c r="T1" s="110"/>
+      <c r="U1" s="110"/>
+      <c r="V1" s="110"/>
+      <c r="W1" s="110"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="111" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" s="112" t="s">
+        <v>104</v>
+      </c>
+      <c r="R2" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="S2" s="112" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" s="112" t="s">
+        <v>112</v>
+      </c>
+      <c r="U2" s="112" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="112" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="108" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="111">
+        <v>40</v>
+      </c>
+      <c r="M3" s="47">
+        <f>L3*$B$2</f>
+        <v>40</v>
+      </c>
+      <c r="N3" s="47">
+        <f>L3*$C$2</f>
+        <v>40</v>
+      </c>
+      <c r="O3" s="47">
+        <f>M3*(1-$E$5)</f>
+        <v>40</v>
+      </c>
+      <c r="P3" s="47">
+        <f>N3*(1-$E$5)</f>
+        <v>40</v>
+      </c>
+      <c r="Q3" s="47">
+        <f>(O3/P4)^$E$2</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="R3" s="47">
+        <f>MEDIAN(0,Q4,1)</f>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="S3" s="47" t="b">
+        <f>IF(1-R3&lt;$E$8,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="T3" s="47" t="b">
+        <f>IF(R3&lt;$E$8,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="47">
+        <f>L3-INT(R3*L3)</f>
+        <v>26</v>
+      </c>
+      <c r="V3" s="47">
+        <f>IF(S3,IF(T3,L3,U3),0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="K4" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="111">
+        <v>20</v>
+      </c>
+      <c r="M4" s="47">
+        <f>$B$2*L4</f>
+        <v>20</v>
+      </c>
+      <c r="N4" s="47">
+        <f>L4*$C$2</f>
+        <v>20</v>
+      </c>
+      <c r="O4" s="47">
+        <f>M4</f>
+        <v>20</v>
+      </c>
+      <c r="P4" s="47">
+        <f>N4</f>
+        <v>20</v>
+      </c>
+      <c r="Q4" s="47">
+        <f>(O4/P3)^$E$2</f>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="R4" s="47">
+        <f>MEDIAN(0,Q3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="S4" s="47" t="b">
+        <f>IF(1-R4&lt;$E$8,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="47" t="b">
+        <f>IF(R4&lt;$E$8,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="47">
+        <f>L4-INT(R4*L4)</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="47">
+        <f>IF(S4,IF(T4,L4,U4),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="82">
+        <v>0</v>
+      </c>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E7" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E8" s="82">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="K8" s="109" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="110"/>
+      <c r="U8" s="110"/>
+      <c r="V8" s="110"/>
+      <c r="W8" s="110"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K9" s="47"/>
+      <c r="L9" s="111" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="O9" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="P9" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q9" s="112" t="s">
+        <v>104</v>
+      </c>
+      <c r="R9" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="S9" s="112" t="s">
+        <v>109</v>
+      </c>
+      <c r="T9" s="112" t="s">
+        <v>112</v>
+      </c>
+      <c r="U9" s="112" t="s">
+        <v>110</v>
+      </c>
+      <c r="V9" s="112" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K10" s="108" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="111">
+        <v>40</v>
+      </c>
+      <c r="M10" s="47">
+        <f>L10*$B$2</f>
+        <v>40</v>
+      </c>
+      <c r="N10" s="47">
+        <f>L10*$C$2</f>
+        <v>40</v>
+      </c>
+      <c r="O10" s="47">
+        <f>M10*(1-$E$5)</f>
+        <v>40</v>
+      </c>
+      <c r="P10" s="47">
+        <f>N10*(1-$E$5)</f>
+        <v>40</v>
+      </c>
+      <c r="Q10" s="47">
+        <f>(O10/P11)^$E$2</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="R10" s="47">
+        <f>MEDIAN(0,Q11,1)</f>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="S10" s="47" t="b">
+        <f>IF(1-R10&lt;$E$8,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="T10" s="47" t="b">
+        <f>IF(R10&lt;$E$8,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="47">
+        <f>L10-INT(R10*L10)</f>
+        <v>26</v>
+      </c>
+      <c r="V10" s="47">
+        <f>IF(S10,IF(T10,L10,U10),0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K11" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11" s="111">
+        <v>20</v>
+      </c>
+      <c r="M11" s="47">
+        <f>$B$2*L11</f>
+        <v>20</v>
+      </c>
+      <c r="N11" s="47">
+        <f>L11*$C$2</f>
+        <v>20</v>
+      </c>
+      <c r="O11" s="47">
+        <f>M11</f>
+        <v>20</v>
+      </c>
+      <c r="P11" s="47">
+        <f>N11</f>
+        <v>20</v>
+      </c>
+      <c r="Q11" s="47">
+        <f>(O11/P10)^$E$2</f>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="R11" s="47">
+        <f>MEDIAN(0,Q10,1)</f>
+        <v>1</v>
+      </c>
+      <c r="S11" s="47" t="b">
+        <f>IF(1-R11&lt;$E$8,FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="47" t="b">
+        <f>IF(R11&lt;$E$8,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="47">
+        <f>L11-INT(R11*L11)</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="47">
+        <f>IF(S11,IF(T11,L11,U11),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="K8:W8"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="K1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550AAB3F-C06C-4BC4-BC52-26C567DF5A60}">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -4242,100 +4723,100 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="86"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="88"/>
       <c r="N1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="88"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="90"/>
       <c r="N2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="88"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="90"/>
       <c r="N3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="88"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="90"/>
       <c r="N4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="88"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="90"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="83"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4350,7 +4831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA015092-742B-4B09-B582-52072BAD5DCA}">
   <dimension ref="G1:L9"/>
   <sheetViews>
@@ -4364,10 +4845,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="80"/>
+      <c r="H1" s="82"/>
       <c r="K1" t="s">
         <v>53</v>
       </c>
@@ -4450,7 +4931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F995D2-727F-4F0D-94D8-60C72D5EAEAA}">
   <dimension ref="A1:AM31"/>
   <sheetViews>
@@ -4555,93 +5036,93 @@
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
-      <c r="T3" s="92"/>
-      <c r="U3" s="92"/>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="96" t="s">
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
+      <c r="S3" s="94"/>
+      <c r="T3" s="94"/>
+      <c r="U3" s="94"/>
+      <c r="V3" s="94"/>
+      <c r="W3" s="94"/>
+      <c r="X3" s="94"/>
+      <c r="Y3" s="94"/>
+      <c r="Z3" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="96"/>
-      <c r="AB3" s="96"/>
-      <c r="AC3" s="96"/>
+      <c r="AA3" s="99"/>
+      <c r="AB3" s="99"/>
+      <c r="AC3" s="99"/>
       <c r="AD3" s="19"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
       <c r="J4" s="25"/>
-      <c r="K4" s="92" t="s">
+      <c r="K4" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
       <c r="O4" s="25"/>
-      <c r="P4" s="92" t="s">
+      <c r="P4" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
-      <c r="S4" s="92"/>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
       <c r="T4" s="25"/>
-      <c r="U4" s="92" t="s">
+      <c r="U4" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92"/>
-      <c r="X4" s="92"/>
-      <c r="Y4" s="84"/>
-      <c r="Z4" s="96" t="s">
+      <c r="V4" s="94"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="96" t="s">
+      <c r="AA4" s="99"/>
+      <c r="AB4" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="AC4" s="96"/>
-      <c r="AD4" s="92" t="s">
+      <c r="AC4" s="99"/>
+      <c r="AD4" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="AE4" s="92"/>
-      <c r="AF4" s="92"/>
-      <c r="AG4" s="92"/>
-      <c r="AH4" s="92"/>
-      <c r="AI4" s="92" t="s">
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="92"/>
-      <c r="AL4" s="92"/>
-      <c r="AM4" s="92"/>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="94"/>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
@@ -4813,85 +5294,85 @@
       <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="102" t="s">
+      <c r="F8" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="103"/>
-      <c r="X8" s="103"/>
-      <c r="Y8" s="104"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="106"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="106"/>
+      <c r="O8" s="106"/>
+      <c r="P8" s="106"/>
+      <c r="Q8" s="106"/>
+      <c r="R8" s="106"/>
+      <c r="S8" s="106"/>
+      <c r="T8" s="106"/>
+      <c r="U8" s="106"/>
+      <c r="V8" s="106"/>
+      <c r="W8" s="106"/>
+      <c r="X8" s="106"/>
+      <c r="Y8" s="107"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="97" t="s">
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="97" t="s">
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="99"/>
-      <c r="P9" s="97" t="s">
+      <c r="L9" s="101"/>
+      <c r="M9" s="101"/>
+      <c r="N9" s="101"/>
+      <c r="O9" s="102"/>
+      <c r="P9" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="98"/>
-      <c r="R9" s="98"/>
-      <c r="S9" s="98"/>
-      <c r="T9" s="99"/>
-      <c r="U9" s="100" t="s">
+      <c r="Q9" s="101"/>
+      <c r="R9" s="101"/>
+      <c r="S9" s="101"/>
+      <c r="T9" s="102"/>
+      <c r="U9" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="101"/>
-      <c r="W9" s="101"/>
-      <c r="X9" s="101"/>
-      <c r="Y9" s="101"/>
-      <c r="Z9" s="93" t="s">
+      <c r="V9" s="104"/>
+      <c r="W9" s="104"/>
+      <c r="X9" s="104"/>
+      <c r="Y9" s="104"/>
+      <c r="Z9" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="94"/>
-      <c r="AB9" s="94"/>
-      <c r="AC9" s="95"/>
-      <c r="AD9" s="89" t="s">
+      <c r="AA9" s="97"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="98"/>
+      <c r="AD9" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="AE9" s="90"/>
-      <c r="AF9" s="90"/>
-      <c r="AG9" s="90"/>
-      <c r="AH9" s="91"/>
-      <c r="AI9" s="89" t="s">
+      <c r="AE9" s="92"/>
+      <c r="AF9" s="92"/>
+      <c r="AG9" s="92"/>
+      <c r="AH9" s="95"/>
+      <c r="AI9" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="AJ9" s="90"/>
-      <c r="AK9" s="90"/>
-      <c r="AL9" s="90"/>
-      <c r="AM9" s="91"/>
+      <c r="AJ9" s="92"/>
+      <c r="AK9" s="92"/>
+      <c r="AL9" s="92"/>
+      <c r="AM9" s="95"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
@@ -7677,11 +8158,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="P4:S4"/>
     <mergeCell ref="AI9:AM9"/>
     <mergeCell ref="AD9:AH9"/>
     <mergeCell ref="AD4:AH4"/>
@@ -7697,6 +8173,11 @@
     <mergeCell ref="P9:T9"/>
     <mergeCell ref="U9:Y9"/>
     <mergeCell ref="F8:Y8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="P4:S4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
api sends all action troop tasks to the game, frontend shows enemy troop actions by red color
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitd\minute_empire\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9E21CD-B383-4B5D-B15E-6B22B5E5F78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48451854-BF5D-4582-B0DC-78F3BAF4BD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="120">
   <si>
     <t>Collections</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>Penaly:</t>
+  </si>
+  <si>
+    <t>Case 2 - Militia vs Archer (Archer defending)</t>
   </si>
 </sst>
 </file>
@@ -1392,15 +1395,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1435,6 +1435,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4315,10 +4318,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139C9724-4F9F-4074-A497-A1553C1D940C}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4717,21 +4720,6 @@
       <c r="D15" s="84"/>
       <c r="E15" s="84"/>
       <c r="F15" s="84"/>
-      <c r="K15" s="85" t="s">
-        <v>114</v>
-      </c>
-      <c r="L15" s="86"/>
-      <c r="M15" s="86"/>
-      <c r="N15" s="86"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="86"/>
-      <c r="Q15" s="86"/>
-      <c r="R15" s="86"/>
-      <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
-      <c r="U15" s="86"/>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" s="84" t="s">
@@ -4741,42 +4729,8 @@
       <c r="D16" s="84"/>
       <c r="E16" s="84"/>
       <c r="F16" s="84"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="83" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="N16" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="O16" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="P16" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q16" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="R16" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="S16" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="T16" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="U16" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="V16" s="47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>117</v>
       </c>
@@ -4786,54 +4740,8 @@
       <c r="D17" t="s">
         <v>118</v>
       </c>
-      <c r="K17" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="L17" s="83">
-        <v>40</v>
-      </c>
-      <c r="M17" s="47">
-        <f>L17*$B$2</f>
-        <v>40</v>
-      </c>
-      <c r="N17" s="47">
-        <f>L17*$C$2</f>
-        <v>40</v>
-      </c>
-      <c r="O17" s="47">
-        <f>M17*(1-D18)</f>
-        <v>24</v>
-      </c>
-      <c r="P17" s="47">
-        <f>N17*(1-D18)</f>
-        <v>24</v>
-      </c>
-      <c r="Q17" s="47">
-        <f>(O17/P18)^$E$2</f>
-        <v>1.3145341380123987</v>
-      </c>
-      <c r="R17" s="47">
-        <f>MEDIAN(0,Q18,1)</f>
-        <v>0.7607257743127307</v>
-      </c>
-      <c r="S17" s="47" t="b">
-        <f>IF(1-R17&lt;$E$8,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="T17" s="47" t="b">
-        <f>IF(R17&lt;$E$8,TRUE,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U17" s="47">
-        <f>L17-INT(R17*L17)</f>
-        <v>10</v>
-      </c>
-      <c r="V17" s="47">
-        <f>IF(S17,IF(T17,L17,U17),0)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>100</v>
       </c>
@@ -4844,54 +4752,8 @@
         <f>B18*0.2/C18</f>
         <v>0.4</v>
       </c>
-      <c r="K18" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="L18" s="83">
-        <v>20</v>
-      </c>
-      <c r="M18" s="47">
-        <f>$B$2*L18</f>
-        <v>20</v>
-      </c>
-      <c r="N18" s="47">
-        <f>L18*$C$2</f>
-        <v>20</v>
-      </c>
-      <c r="O18" s="47">
-        <f>M18</f>
-        <v>20</v>
-      </c>
-      <c r="P18" s="47">
-        <f>N18</f>
-        <v>20</v>
-      </c>
-      <c r="Q18" s="47">
-        <f>(O18/P17)^$E$2</f>
-        <v>0.7607257743127307</v>
-      </c>
-      <c r="R18" s="47">
-        <f>MEDIAN(0,Q17,1)</f>
-        <v>1</v>
-      </c>
-      <c r="S18" s="47" t="b">
-        <f>IF(1-R18&lt;$E$8,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="T18" s="47" t="b">
-        <f>IF(R18&lt;$E$8,TRUE,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U18" s="47">
-        <f>L18-INT(R18*L18)</f>
-        <v>0</v>
-      </c>
-      <c r="V18" s="47">
-        <f>IF(S18,IF(T18,L18,U18),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>50</v>
       </c>
@@ -4903,7 +4765,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>10</v>
       </c>
@@ -4915,19 +4777,167 @@
         <v>0.04</v>
       </c>
     </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K21" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="86"/>
+      <c r="R21" s="86"/>
+      <c r="S21" s="86"/>
+      <c r="T21" s="86"/>
+      <c r="U21" s="86"/>
+      <c r="V21" s="86"/>
+      <c r="W21" s="86"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K22" s="47"/>
+      <c r="L22" s="83" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="N22" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="O22" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="P22" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q22" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="R22" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="S22" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="T22" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="U22" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="V22" s="47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K23" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" s="83">
+        <v>8</v>
+      </c>
+      <c r="M23" s="47">
+        <f>L23*$B$2</f>
+        <v>8</v>
+      </c>
+      <c r="N23" s="47">
+        <f>L23*$C$3</f>
+        <v>4</v>
+      </c>
+      <c r="O23" s="47">
+        <f>M23*(1-D24)</f>
+        <v>8</v>
+      </c>
+      <c r="P23" s="47">
+        <f>N23*(1-D24)</f>
+        <v>4</v>
+      </c>
+      <c r="Q23" s="47">
+        <f>(O23/P24)^$E$2</f>
+        <v>0.71554175279993271</v>
+      </c>
+      <c r="R23" s="47">
+        <f>MEDIAN(0,Q24,1)</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="47" t="b">
+        <f>IF(1-R23&lt;$E$8,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="T23" s="47" t="b">
+        <f>IF(R23&lt;$E$8,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="U23" s="47">
+        <f>L23-INT(R23*L23)</f>
+        <v>8</v>
+      </c>
+      <c r="V23" s="47">
+        <f>IF(S23,IF(T23,L23,U23),0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K24" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="L24" s="83">
+        <v>20</v>
+      </c>
+      <c r="M24" s="47">
+        <v>0</v>
+      </c>
+      <c r="N24" s="47">
+        <f>L24*$C$3</f>
+        <v>10</v>
+      </c>
+      <c r="O24" s="47">
+        <f>M24</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="47">
+        <f>N24</f>
+        <v>10</v>
+      </c>
+      <c r="Q24" s="47">
+        <f>(O24/P23)^$E$2</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="47">
+        <f>MEDIAN(0,Q23,1)</f>
+        <v>0.71554175279993271</v>
+      </c>
+      <c r="S24" s="47" t="b">
+        <f>IF(1-R24&lt;$E$8,FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="T24" s="47" t="b">
+        <f>IF(R24&lt;$E$8,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="47">
+        <f>L24-INT(R24*L24)</f>
+        <v>6</v>
+      </c>
+      <c r="V24" s="47">
+        <f>IF(S24,IF(T24,L24,U24),0)</f>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="K21:W21"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="K8:W8"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="K1:W1"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="K8:W8"/>
-    <mergeCell ref="K15:W15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5279,12 +5289,12 @@
       <c r="W3" s="98"/>
       <c r="X3" s="98"/>
       <c r="Y3" s="98"/>
-      <c r="Z3" s="103" t="s">
+      <c r="Z3" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="103"/>
-      <c r="AB3" s="103"/>
-      <c r="AC3" s="103"/>
+      <c r="AA3" s="102"/>
+      <c r="AB3" s="102"/>
+      <c r="AC3" s="102"/>
       <c r="AD3" s="19"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -5322,14 +5332,14 @@
       <c r="W4" s="98"/>
       <c r="X4" s="98"/>
       <c r="Y4" s="90"/>
-      <c r="Z4" s="103" t="s">
+      <c r="Z4" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" s="103"/>
-      <c r="AB4" s="103" t="s">
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="AC4" s="103"/>
+      <c r="AC4" s="102"/>
       <c r="AD4" s="98" t="s">
         <v>82</v>
       </c>
@@ -5515,28 +5525,28 @@
       <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="109" t="s">
+      <c r="F8" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="110"/>
-      <c r="S8" s="110"/>
-      <c r="T8" s="110"/>
-      <c r="U8" s="110"/>
-      <c r="V8" s="110"/>
-      <c r="W8" s="110"/>
-      <c r="X8" s="110"/>
-      <c r="Y8" s="111"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="109"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="109"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="109"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="109"/>
+      <c r="V8" s="109"/>
+      <c r="W8" s="109"/>
+      <c r="X8" s="109"/>
+      <c r="Y8" s="110"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
@@ -5545,55 +5555,55 @@
       </c>
       <c r="C9" s="96"/>
       <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="104" t="s">
+      <c r="E9" s="111"/>
+      <c r="F9" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="104" t="s">
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="104" t="s">
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
-      <c r="S9" s="105"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="107" t="s">
+      <c r="Q9" s="104"/>
+      <c r="R9" s="104"/>
+      <c r="S9" s="104"/>
+      <c r="T9" s="105"/>
+      <c r="U9" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="108"/>
-      <c r="W9" s="108"/>
-      <c r="X9" s="108"/>
-      <c r="Y9" s="108"/>
-      <c r="Z9" s="100" t="s">
+      <c r="V9" s="107"/>
+      <c r="W9" s="107"/>
+      <c r="X9" s="107"/>
+      <c r="Y9" s="107"/>
+      <c r="Z9" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="101"/>
-      <c r="AB9" s="101"/>
-      <c r="AC9" s="102"/>
+      <c r="AA9" s="100"/>
+      <c r="AB9" s="100"/>
+      <c r="AC9" s="101"/>
       <c r="AD9" s="95" t="s">
         <v>81</v>
       </c>
       <c r="AE9" s="96"/>
       <c r="AF9" s="96"/>
       <c r="AG9" s="96"/>
-      <c r="AH9" s="99"/>
+      <c r="AH9" s="97"/>
       <c r="AI9" s="95" t="s">
         <v>80</v>
       </c>
       <c r="AJ9" s="96"/>
       <c r="AK9" s="96"/>
       <c r="AL9" s="96"/>
-      <c r="AM9" s="99"/>
+      <c r="AM9" s="97"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
@@ -8379,6 +8389,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="P4:S4"/>
     <mergeCell ref="AI9:AM9"/>
     <mergeCell ref="AD9:AH9"/>
     <mergeCell ref="AD4:AH4"/>
@@ -8394,11 +8409,6 @@
     <mergeCell ref="P9:T9"/>
     <mergeCell ref="U9:Y9"/>
     <mergeCell ref="F8:Y8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="P4:S4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
balance werehouse storage capacity
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitd\minute_empire\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48451854-BF5D-4582-B0DC-78F3BAF4BD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2522C2-2C13-4BCD-B215-37E0EA6C17C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{BCAE3296-52B4-4992-8D47-6E2C2F757A90}"/>
   </bookViews>
   <sheets>
     <sheet name="brainstorming" sheetId="1" r:id="rId1"/>
@@ -1395,12 +1395,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1435,9 +1438,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4320,7 +4320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139C9724-4F9F-4074-A497-A1553C1D940C}">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
@@ -4927,17 +4927,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="K1:W1"/>
     <mergeCell ref="K21:W21"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="K8:W8"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="K1:W1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5166,9 +5166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F995D2-727F-4F0D-94D8-60C72D5EAEAA}">
   <dimension ref="A1:AM31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD31" sqref="AD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5289,12 +5289,12 @@
       <c r="W3" s="98"/>
       <c r="X3" s="98"/>
       <c r="Y3" s="98"/>
-      <c r="Z3" s="102" t="s">
+      <c r="Z3" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="102"/>
-      <c r="AB3" s="102"/>
-      <c r="AC3" s="102"/>
+      <c r="AA3" s="103"/>
+      <c r="AB3" s="103"/>
+      <c r="AC3" s="103"/>
       <c r="AD3" s="19"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -5332,14 +5332,14 @@
       <c r="W4" s="98"/>
       <c r="X4" s="98"/>
       <c r="Y4" s="90"/>
-      <c r="Z4" s="102" t="s">
+      <c r="Z4" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="AA4" s="102"/>
-      <c r="AB4" s="102" t="s">
+      <c r="AA4" s="103"/>
+      <c r="AB4" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="AC4" s="102"/>
+      <c r="AC4" s="103"/>
       <c r="AD4" s="98" t="s">
         <v>82</v>
       </c>
@@ -5525,28 +5525,28 @@
       <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="108" t="s">
+      <c r="F8" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-      <c r="N8" s="109"/>
-      <c r="O8" s="109"/>
-      <c r="P8" s="109"/>
-      <c r="Q8" s="109"/>
-      <c r="R8" s="109"/>
-      <c r="S8" s="109"/>
-      <c r="T8" s="109"/>
-      <c r="U8" s="109"/>
-      <c r="V8" s="109"/>
-      <c r="W8" s="109"/>
-      <c r="X8" s="109"/>
-      <c r="Y8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="110"/>
+      <c r="U8" s="110"/>
+      <c r="V8" s="110"/>
+      <c r="W8" s="110"/>
+      <c r="X8" s="110"/>
+      <c r="Y8" s="111"/>
     </row>
     <row r="9" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
@@ -5555,55 +5555,55 @@
       </c>
       <c r="C9" s="96"/>
       <c r="D9" s="96"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="103" t="s">
+      <c r="E9" s="97"/>
+      <c r="F9" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="103" t="s">
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="104"/>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="103" t="s">
+      <c r="L9" s="105"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="106"/>
+      <c r="P9" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="104"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="T9" s="105"/>
-      <c r="U9" s="106" t="s">
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
+      <c r="S9" s="105"/>
+      <c r="T9" s="106"/>
+      <c r="U9" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="107"/>
-      <c r="W9" s="107"/>
-      <c r="X9" s="107"/>
-      <c r="Y9" s="107"/>
-      <c r="Z9" s="99" t="s">
+      <c r="V9" s="108"/>
+      <c r="W9" s="108"/>
+      <c r="X9" s="108"/>
+      <c r="Y9" s="108"/>
+      <c r="Z9" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="100"/>
-      <c r="AB9" s="100"/>
-      <c r="AC9" s="101"/>
+      <c r="AA9" s="101"/>
+      <c r="AB9" s="101"/>
+      <c r="AC9" s="102"/>
       <c r="AD9" s="95" t="s">
         <v>81</v>
       </c>
       <c r="AE9" s="96"/>
       <c r="AF9" s="96"/>
       <c r="AG9" s="96"/>
-      <c r="AH9" s="97"/>
+      <c r="AH9" s="99"/>
       <c r="AI9" s="95" t="s">
         <v>80</v>
       </c>
       <c r="AJ9" s="96"/>
       <c r="AK9" s="96"/>
       <c r="AL9" s="96"/>
-      <c r="AM9" s="97"/>
+      <c r="AM9" s="99"/>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
@@ -6266,7 +6266,7 @@
         <v>1323.2831999999996</v>
       </c>
       <c r="AA14" s="19">
-        <f t="shared" si="14"/>
+        <f>$AC$5*($AC$6^($A14))</f>
         <v>1323.2831999999996</v>
       </c>
       <c r="AB14" s="19">
@@ -8389,11 +8389,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="P4:S4"/>
     <mergeCell ref="AI9:AM9"/>
     <mergeCell ref="AD9:AH9"/>
     <mergeCell ref="AD4:AH4"/>
@@ -8409,6 +8404,11 @@
     <mergeCell ref="P9:T9"/>
     <mergeCell ref="U9:Y9"/>
     <mergeCell ref="F8:Y8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="P4:S4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>